<commit_message>
Updated with more areas.
</commit_message>
<xml_diff>
--- a/data/data_vuv.xlsx
+++ b/data/data_vuv.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="289">
   <si>
     <t xml:space="preserve">VarName1</t>
   </si>
@@ -312,6 +312,9 @@
     <t xml:space="preserve">W at 63.02. Strong W event at 59.92s (with some Cu). Cu event at 61.94s.</t>
   </si>
   <si>
+    <t xml:space="preserve">BEION4/Divertor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ti from pickup coil near UDPT</t>
   </si>
   <si>
@@ -354,9 +357,6 @@
     <t xml:space="preserve">W event at 54.06s. Followed by a series of larger W events until disruption at 54.56s</t>
   </si>
   <si>
-    <t xml:space="preserve">BEION4/Divertor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Small one.</t>
   </si>
   <si>
@@ -366,6 +366,9 @@
     <t xml:space="preserve">(371, 474)</t>
   </si>
   <si>
+    <t xml:space="preserve">BEION4/LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">UFO seen coming from the divertor in the bottom right part of the image, that corresponds to a increase on radiated light as SL says.</t>
   </si>
   <si>
@@ -418,6 +421,9 @@
   </si>
   <si>
     <t xml:space="preserve">No specific influxes. Spectrum dominated by Ne emission during plasma termination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH/NPL</t>
   </si>
   <si>
     <t xml:space="preserve">Huge UFO appeared on UDPT but smaller UFOs begun to appear as early as around 48.75s.(very likely Ti according to JETDSP).</t>
@@ -550,9 +556,6 @@
     <t xml:space="preserve">UFO inner divertor seen for ~ 5 frames</t>
   </si>
   <si>
-    <t xml:space="preserve">With this camera is the UFOs are  visible but cannot be tracked.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Either it appears and disappears or there are different. I annotated the mean speed (which seems to be similar)</t>
   </si>
   <si>
@@ -605,7 +608,10 @@
     <t xml:space="preserve">Clear Mo influx at 5.68s</t>
   </si>
   <si>
-    <t xml:space="preserve">Large UFO falls from near upper inner sausages</t>
+    <t xml:space="preserve">Divertor/ILA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large UFO falls from near upper inner sausages. Makred as BEIOn4 – as I can’t see the equivalence in this camera on the wiki.</t>
   </si>
   <si>
     <t xml:space="preserve">Nice tracking of the big one. There are other UFO (smaller) in the video.</t>
@@ -626,6 +632,9 @@
     <t xml:space="preserve">(221, 83)</t>
   </si>
   <si>
+    <t xml:space="preserve">LH/NPL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frames: 1320-1347 (Inner side during the termination phase)</t>
   </si>
   <si>
@@ -647,6 +656,9 @@
     <t xml:space="preserve">(122, 163)</t>
   </si>
   <si>
+    <t xml:space="preserve">LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Very bright UFO falling vertically. Apparently the cause of radiation spike.</t>
   </si>
   <si>
@@ -683,18 +695,15 @@
     <t xml:space="preserve">A spot appears in experimental camera (Be II filter) near top of machine for two frames, about 60 ms before disruption.</t>
   </si>
   <si>
-    <t xml:space="preserve">Could not find the spot, but tracked two other UFOs (see below); this one at t = 49.65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(115, 26)</t>
+    <t xml:space="preserve">More UFOs near 49.8s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(99, 46)</t>
   </si>
   <si>
     <t xml:space="preserve">As yet unidentified impurity for 1 frame at 50.36s</t>
   </si>
   <si>
-    <t xml:space="preserve">(99, 46)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Apparently material coming out of the lower corner of ILA --&gt; Be signal in spectroscopy observed as well</t>
   </si>
   <si>
@@ -770,6 +779,9 @@
     <t xml:space="preserve">Very messy plasma. VUV spectrum mostly saturated at this time.</t>
   </si>
   <si>
+    <t xml:space="preserve">UIWP/IWGL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stereographic UFO view after rough landing.</t>
   </si>
   <si>
@@ -870,6 +882,15 @@
   </si>
   <si>
     <t xml:space="preserve">Not trackable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame: 329 Time: 51.186s  Titanium influx confirmed by spectroscopy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(539, 186)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDT</t>
   </si>
 </sst>
 </file>
@@ -880,7 +901,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -907,6 +928,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -951,7 +977,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -966,6 +992,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -995,13 +1025,13 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="15600" ySplit="0" topLeftCell="A45" activePane="topLeft" state="split"/>
-      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
-      <selection pane="topRight" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="16419" ySplit="0" topLeftCell="A55" activePane="topLeft" state="split"/>
+      <selection pane="topLeft" activeCell="I48" activeCellId="0" sqref="I48"/>
+      <selection pane="topRight" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.18"/>
@@ -1763,6 +1793,9 @@
       <c r="L19" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="M19" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1784,19 +1817,19 @@
         <v>50.986</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>-999</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K20" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M20" s="0" t="s">
         <v>23</v>
@@ -1822,22 +1855,25 @@
         <v>50.718</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,22 +1896,25 @@
         <v>50.846</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>12511</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,22 +1937,22 @@
         <v>54.275</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>-999</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,6 +1992,9 @@
       <c r="L24" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="M24" s="0" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -1974,22 +2016,25 @@
         <v>43.664</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>2604</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,13 +2060,13 @@
         <v>-999</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K26" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M26" s="0" t="s">
         <v>56</v>
@@ -2047,22 +2092,22 @@
         <v>48.565</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>839</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M27" s="0" t="s">
         <v>61</v>
@@ -2088,22 +2133,25 @@
         <v>47.787</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1412</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K28" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2120,25 +2168,28 @@
         <v>54.1327</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>54.159</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>-999</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>77</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,22 +2212,25 @@
         <v>50.908</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K30" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,19 +2253,19 @@
         <v>56.252</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>1111</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K31" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="M31" s="0" t="s">
         <v>23</v>
@@ -2237,19 +2291,22 @@
         <v>52.155</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="M32" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2272,19 +2329,19 @@
         <v>59.429</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>-999</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K33" s="0" t="s">
         <v>77</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M33" s="0" t="s">
         <v>23</v>
@@ -2310,22 +2367,22 @@
         <v>50.105</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>684</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K34" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M34" s="0" t="s">
         <v>23</v>
@@ -2351,22 +2408,22 @@
         <v>42.667</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>1073</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M35" s="0" t="s">
         <v>61</v>
@@ -2392,22 +2449,22 @@
         <v>50.436</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K36" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="M36" s="0" t="s">
         <v>23</v>
@@ -2433,7 +2490,7 @@
         <v>63.443</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>0</v>
@@ -2442,13 +2499,16 @@
         <v>112</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>26</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,22 +2531,22 @@
         <v>63.059</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K38" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="M38" s="0" t="s">
         <v>23</v>
@@ -2512,22 +2572,22 @@
         <v>58.143</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="M39" s="0" t="s">
         <v>23</v>
@@ -2553,25 +2613,25 @@
         <v>58.16</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>743.3</v>
       </c>
       <c r="I40" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J40" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="M40" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,24 +2654,24 @@
         <v>55.644</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>-999</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K41" s="0" t="s">
         <v>77</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>2070</v>
+        <v>2071</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>101237</v>
@@ -2623,19 +2683,19 @@
         <v>47.299</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>61.057</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>2718</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K42" s="0" t="s">
         <v>26</v>
@@ -2643,305 +2703,332 @@
       <c r="L42" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="M42" s="0" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>2071</v>
+        <v>2128</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>101237</v>
+        <v>100549</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>47.299</v>
+        <v>51.068</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>61.057</v>
+        <v>0</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H43" s="0" t="n">
-        <v>2718</v>
+        <v>4240</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>180</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>181</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>2128</v>
+        <v>2132</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>100549</v>
+        <v>100395</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>51.068</v>
+        <v>54.7</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>177</v>
+        <v>65.683</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>4240</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>179</v>
+        <v>-999</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>2132</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>100395</v>
+        <v>2165</v>
+      </c>
+      <c r="B45" s="4" t="n">
+        <v>103559</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>54.7</v>
+        <v>50.22336</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>65.683</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>182</v>
+        <v>50.551</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>186</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>-999</v>
+        <v>1929</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
+      </c>
+      <c r="M45" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>2165</v>
+        <v>2170</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>103559</v>
+        <v>101432</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>50.22336</v>
+        <v>51.699</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>50.551</v>
+        <v>55.845</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>1929</v>
+        <v>4927.1</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>191</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>193</v>
+      </c>
+      <c r="M46" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>2170</v>
+        <v>2171</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>101432</v>
+        <v>101282</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>51.699</v>
+        <v>63.87473</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>55.845</v>
+        <v>63.073</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>4927.1</v>
+        <v>4291.5</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+      <c r="M47" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>2171</v>
+        <v>2178</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>101282</v>
+        <v>99902</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>63.87473</v>
+        <v>55.0125</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>184</v>
+        <v>13</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>63.073</v>
+        <v>55.179</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>4291.5</v>
+        <v>1814</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>196</v>
+        <v>27</v>
+      </c>
+      <c r="M48" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>2178</v>
+        <v>2183</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>99902</v>
+        <v>99811</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>55.0125</v>
+        <v>55.512</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>55.179</v>
+        <v>55.52</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>1814</v>
+        <v>-999</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>27</v>
+        <v>206</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>2183</v>
+        <v>2184</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>99811</v>
+        <v>99802</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>55.512</v>
+        <v>47.4125</v>
       </c>
       <c r="E50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>55.52</v>
+        <v>49.021</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>203</v>
+        <v>27</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>2184</v>
+        <v>2185</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>99802</v>
@@ -2950,7 +3037,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>47.4125</v>
+        <v>48.0875</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>13</v>
@@ -2959,779 +3046,794 @@
         <v>49.021</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>0</v>
+        <v>7121</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>27</v>
+        <v>214</v>
+      </c>
+      <c r="M51" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>2185</v>
+        <v>2209</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>99802</v>
+        <v>99513</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>48.0875</v>
+        <v>50.8875</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>49.021</v>
+        <v>51.659</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>7121</v>
+        <v>0</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="K52" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>2232</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>99205</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>48.76</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>48.945</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>908</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="K53" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="M52" s="0" t="s">
+      <c r="L53" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M53" s="0" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>2209</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>99513</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>50.8875</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>51.659</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="K53" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>2232</v>
+        <v>2242</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>99205</v>
+        <v>97487</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>48.76</v>
+        <v>50.35</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>48.945</v>
+        <v>50.417</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>908</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>215</v>
+        <v>663</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="M54" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>2242</v>
+        <v>2266</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>97487</v>
+        <v>96361</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>50.35</v>
+        <v>54.85</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>50.417</v>
+        <v>56.096</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="H55" s="0" t="n">
-        <v>1082</v>
+        <v>0</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="J55" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>221</v>
+        <v>27</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>2242</v>
+        <v>2289</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>97487</v>
+        <v>103802</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>50.35</v>
+        <v>55.722</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>50.417</v>
+        <v>55.807</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="H56" s="0" t="n">
-        <v>663</v>
+        <v>1131</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>229</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>231</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>2266</v>
+        <v>2294</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>96361</v>
+        <v>102879</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>54.85</v>
+        <v>47.9852</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>56.096</v>
+        <v>47.985</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>0</v>
+        <v>9013</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>224</v>
+        <v>233</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>234</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>235</v>
+      </c>
+      <c r="M57" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>2289</v>
+        <v>2308</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>103802</v>
+        <v>101433</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>55.722</v>
+        <v>56.2625</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>128</v>
+        <v>13</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>55.807</v>
+        <v>56.403</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="H58" s="0" t="n">
-        <v>1131</v>
+        <v>-999</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>54</v>
+        <v>240</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
       <c r="M58" s="0" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>2294</v>
+        <v>2321</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>102879</v>
+        <v>100210</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>47.9852</v>
+        <v>54.1625</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>47.985</v>
+        <v>54.218</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="H59" s="0" t="n">
-        <v>9013</v>
+        <v>5672</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="K59" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="M59" s="0" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>2308</v>
+        <v>2322</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>101433</v>
+        <v>100208</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>56.2625</v>
+        <v>52.5875</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>56.403</v>
+        <v>52.75</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>-999</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>173</v>
+        <v>250</v>
+      </c>
+      <c r="M60" s="0" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>2321</v>
+        <v>2323</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>100210</v>
+        <v>100186</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>54.1625</v>
+        <v>57.583</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>54.218</v>
+        <v>0</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>5672</v>
+        <v>2236.067</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="K61" s="0" t="s">
         <v>17</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="M61" s="0" t="s">
-        <v>242</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>2322</v>
+        <v>2324</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>100208</v>
+        <v>100130</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>52.5875</v>
+        <v>53.8851</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>52.75</v>
+        <v>53.925</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="H62" s="0" t="n">
-        <v>-999</v>
+        <v>60075</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="K62" s="0" t="s">
-        <v>246</v>
+        <v>77</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+      <c r="M62" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>2323</v>
+        <v>237</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>100186</v>
+        <v>99381</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D63" s="0" t="n">
-        <v>57.583</v>
+      <c r="D63" s="0" t="s">
+        <v>259</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F63" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F63" s="5" t="n">
+        <v>57458</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>894</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="M63" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>99340</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>49.46257</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G63" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>2236.067</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="K63" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="M63" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>2324</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <v>100130</v>
-      </c>
-      <c r="C64" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D64" s="0" t="n">
-        <v>53.8851</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="0" t="n">
-        <v>53.925</v>
-      </c>
       <c r="G64" s="0" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="H64" s="0" t="n">
-        <v>60075</v>
+        <v>1002</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>237</v>
+        <v>313</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>99381</v>
-      </c>
-      <c r="C65" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>255</v>
+        <v>98992</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>51</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="4" t="n">
-        <v>57458</v>
+      <c r="F65" s="0" t="n">
+        <v>52.957</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="H65" s="0" t="n">
-        <v>894</v>
+        <v>0</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="K65" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="L65" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M65" s="0" t="s">
-        <v>233</v>
+      <c r="L65" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="M65" s="6" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>254</v>
+        <v>382</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>99340</v>
+        <v>98186</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>49.46257</v>
+        <v>45.46594</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>0</v>
+        <v>48.037</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="H66" s="0" t="n">
-        <v>1002</v>
+        <v>-999</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="K66" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="M66" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>98184</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="L66" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="M66" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>313</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <v>98992</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>260</v>
-      </c>
       <c r="D67" s="0" t="n">
-        <v>51</v>
+        <v>45.26628</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>52.957</v>
+        <v>48.038</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>0</v>
+        <v>-999</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>267</v>
+        <v>37</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>54</v>
+        <v>275</v>
       </c>
       <c r="L67" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="M67" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
+      </c>
+      <c r="M67" s="0" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>98186</v>
+        <v>97987</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>45.46594</v>
+        <v>50.18166</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>48.037</v>
+        <v>0</v>
       </c>
       <c r="G68" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="K68" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L68" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="H68" s="0" t="n">
-        <v>-999</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="K68" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="L68" s="0" t="s">
-        <v>265</v>
-      </c>
       <c r="M68" s="0" t="s">
-        <v>272</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>98184</v>
+        <v>97988</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>45.26628</v>
+        <v>50.18</v>
       </c>
       <c r="E69" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>48.038</v>
+        <v>0</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="H69" s="0" t="n">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>37</v>
+        <v>281</v>
       </c>
       <c r="K69" s="0" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="L69" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="M69" s="0" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>408</v>
+        <v>922</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>97987</v>
+        <v>96220</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>50.18166</v>
+        <v>48.61</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J70" s="0" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="K70" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L70" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="M70" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>405</v>
+        <v>1098</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>97988</v>
+        <v>94209</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>50.18</v>
+        <v>49.149</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>13</v>
@@ -3740,59 +3842,29 @@
         <v>0</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="H71" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>277</v>
+        <v>112</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>287</v>
       </c>
       <c r="K71" s="0" t="s">
-        <v>278</v>
+        <v>54</v>
       </c>
       <c r="L71" s="0" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>922</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>96220</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>48.61</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H72" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I72" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="K72" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="L72" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="M72" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
+        <v>269</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Last version. Not sure what's changed tho.
</commit_message>
<xml_diff>
--- a/data/data_vuv.xlsx
+++ b/data/data_vuv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="285">
   <si>
     <t>VarName1</t>
   </si>
@@ -874,6 +874,15 @@
   </si>
   <si>
     <t>Can’t be tracked. There are two at 4D and UDPT The time is tricky as the Opcamera does not have the time vector.</t>
+  </si>
+  <si>
+    <t>Bright flash at the top of the outboard side associated with a titanium signal in KT2.</t>
+  </si>
+  <si>
+    <t>There's yet another UFO right after, not as visible.</t>
+  </si>
+  <si>
+    <t>Based on comment (KT2)</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="17280"/>
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="C44" sqref="C44"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -3642,7 +3651,7 @@
         <v>251</v>
       </c>
       <c r="H61">
-        <v>60075</v>
+        <v>-999</v>
       </c>
       <c r="I61" t="s">
         <v>252</v>
@@ -4012,6 +4021,44 @@
       </c>
       <c r="M70" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>379</v>
+      </c>
+      <c r="B71">
+        <v>97851</v>
+      </c>
+      <c r="C71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D71" s="5">
+        <v>49225</v>
+      </c>
+      <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71" t="s">
+        <v>282</v>
+      </c>
+      <c r="H71">
+        <v>747</v>
+      </c>
+      <c r="I71" t="s">
+        <v>283</v>
+      </c>
+      <c r="K71" t="s">
+        <v>54</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="M71" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bunch of -999 with the GUI
</commit_message>
<xml_diff>
--- a/data/data_vuv.xlsx
+++ b/data/data_vuv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="294">
   <si>
     <t>VarName1</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Large UFO at the inboard side</t>
   </si>
   <si>
-    <t>Analysed E5WE at 48.747</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>UFO's during disruption also seen by KLDT-E5WD</t>
   </si>
   <si>
-    <t>Literally dozens of UFOs over the 50s mark.</t>
-  </si>
-  <si>
     <t>W feature on KT2 saturates at 55.5s. Series of smaller W events starting at 55.18s. Plasma looks to be heading for disruption when these begin.</t>
   </si>
   <si>
@@ -319,9 +313,6 @@
     <t>Ti from pickup coil near UDPT</t>
   </si>
   <si>
-    <t>I don’t see anything on any camera</t>
-  </si>
-  <si>
     <t>Ti event at 49.96s</t>
   </si>
   <si>
@@ -418,9 +409,6 @@
     <t>UFOS coming from outerwall during disruption seen also by KLDT-E5WD camera.</t>
   </si>
   <si>
-    <t>A cloud is visible on the op camera after it already start disrupting, but nothing traceable on the experimental ones.</t>
-  </si>
-  <si>
     <t>No specific influxes. Spectrum dominated by Ne emission during plasma termination.</t>
   </si>
   <si>
@@ -458,9 +446,6 @@
   </si>
   <si>
     <t>Titanium UFO over 2 frames</t>
-  </si>
-  <si>
-    <t>Not visible with exp camera</t>
   </si>
   <si>
     <t>Not conclusive due to domination of spectrum by Ar and Ne  from seeding.</t>
@@ -639,12 +624,6 @@
     <t>Frames: 1320-1347 (Inner side during the termination phase)</t>
   </si>
   <si>
-    <t>Massive cloud of UFOs</t>
-  </si>
-  <si>
-    <t>(215, 304)</t>
-  </si>
-  <si>
     <t>W event at 55.5s</t>
   </si>
   <si>
@@ -883,6 +862,54 @@
   </si>
   <si>
     <t>Based on comment (KT2)</t>
+  </si>
+  <si>
+    <t>Very, very small</t>
+  </si>
+  <si>
+    <t>(108, 74)</t>
+  </si>
+  <si>
+    <t>Massive cloud of UFOs at upper left corner. Also, before that, some TIE near the divertor.</t>
+  </si>
+  <si>
+    <t>(285, 97)</t>
+  </si>
+  <si>
+    <t>Analysed E5WE at 48.747. There are several UFOs in plenty of places.</t>
+  </si>
+  <si>
+    <t>Can’t be tracked - lost in next frame.</t>
+  </si>
+  <si>
+    <t>(246, 75)</t>
+  </si>
+  <si>
+    <t>Literally dozens of UFOs over the 50s mark. At first very mild and located over the divertor. I annotated this due to VUV data and because the plasma was already disrupted for the others.</t>
+  </si>
+  <si>
+    <t>I don’t see anything on any exp camera. Some UFOs in divertor. The Ti can be seen at O5WB.</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>(115, 208)</t>
+  </si>
+  <si>
+    <t>The cloud splits and moves towards the inner wall.</t>
+  </si>
+  <si>
+    <t>Not visible with exp camera: I'll take it as it does not move.</t>
+  </si>
+  <si>
+    <t>Only visible in op camera.</t>
   </si>
 </sst>
 </file>
@@ -1215,11 +1242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H46" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="17280"/>
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="H57" sqref="H57"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -1237,7 +1264,7 @@
     <col min="12" max="12" width="45.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1277,8 +1304,11 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1318,8 +1348,11 @@
       <c r="M2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24</v>
       </c>
@@ -1353,8 +1386,11 @@
       <c r="M3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60</v>
       </c>
@@ -1391,8 +1427,11 @@
       <c r="M4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="N4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>66</v>
       </c>
@@ -1432,8 +1471,11 @@
       <c r="M5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>76</v>
       </c>
@@ -1459,7 +1501,7 @@
         <v>3794.73</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>282</v>
       </c>
       <c r="K6" t="s">
         <v>26</v>
@@ -1468,10 +1510,13 @@
         <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>145</v>
       </c>
@@ -1491,28 +1536,31 @@
         <v>61.036999999999999</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
+        <v>283</v>
+      </c>
+      <c r="J7" t="s">
         <v>37</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>38</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" t="s">
         <v>40</v>
       </c>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>150</v>
       </c>
@@ -1532,28 +1580,28 @@
         <v>58.750999999999998</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8">
         <v>1409</v>
       </c>
       <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>44</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="M8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>162</v>
       </c>
@@ -1573,28 +1621,31 @@
         <v>46.377000000000002</v>
       </c>
       <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <v>3635</v>
+      </c>
+      <c r="I9" t="s">
         <v>47</v>
       </c>
-      <c r="H9">
-        <v>-999</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>48</v>
-      </c>
-      <c r="J9" t="s">
-        <v>49</v>
       </c>
       <c r="K9" t="s">
         <v>17</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>196</v>
       </c>
@@ -1614,28 +1665,28 @@
         <v>50.892000000000003</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
         <v>52</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>53</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" t="s">
         <v>55</v>
       </c>
-      <c r="M10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>231</v>
       </c>
@@ -1655,28 +1706,28 @@
         <v>47.408999999999999</v>
       </c>
       <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11">
+        <v>3535</v>
+      </c>
+      <c r="I11" t="s">
         <v>57</v>
       </c>
-      <c r="H11">
-        <v>-999</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>58</v>
-      </c>
-      <c r="J11" t="s">
-        <v>59</v>
       </c>
       <c r="K11" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" t="s">
         <v>60</v>
       </c>
-      <c r="M11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>345</v>
       </c>
@@ -1696,28 +1747,28 @@
         <v>57.530999999999999</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12">
         <v>6134.5</v>
       </c>
       <c r="I12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" t="s">
         <v>63</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>64</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="M12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>652</v>
       </c>
@@ -1737,25 +1788,25 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13">
+        <v>2096</v>
+      </c>
+      <c r="I13" t="s">
         <v>67</v>
       </c>
-      <c r="H13">
-        <v>-999</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>68</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" t="s">
         <v>70</v>
       </c>
-      <c r="M13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>655</v>
       </c>
@@ -1775,25 +1826,28 @@
         <v>42.408000000000001</v>
       </c>
       <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14">
+        <v>3928</v>
+      </c>
+      <c r="I14" t="s">
         <v>72</v>
       </c>
-      <c r="H14">
-        <v>-999</v>
-      </c>
-      <c r="I14" t="s">
-        <v>73</v>
+      <c r="J14" t="s">
+        <v>284</v>
       </c>
       <c r="K14" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>673</v>
       </c>
@@ -1813,25 +1867,25 @@
         <v>60.258000000000003</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H15">
         <v>3259</v>
       </c>
       <c r="I15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" t="s">
         <v>76</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>681</v>
       </c>
@@ -1851,25 +1905,25 @@
         <v>55.588000000000001</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H16">
-        <v>-999</v>
+        <v>837</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>285</v>
       </c>
       <c r="K16" t="s">
         <v>17</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>731</v>
       </c>
@@ -1889,28 +1943,28 @@
         <v>43.744</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H17">
         <v>1596</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K17" t="s">
         <v>17</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>737</v>
       </c>
@@ -1930,25 +1984,25 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H18">
         <v>-999</v>
       </c>
       <c r="I18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K18" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>932</v>
       </c>
@@ -1968,28 +2022,28 @@
         <v>63.055999999999997</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H19">
         <v>3810</v>
       </c>
       <c r="I19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" t="s">
         <v>91</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>93</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>944</v>
       </c>
@@ -2009,25 +2063,25 @@
         <v>50.985999999999997</v>
       </c>
       <c r="G20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H20">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>97</v>
+        <v>286</v>
       </c>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>947</v>
       </c>
@@ -2047,28 +2101,28 @@
         <v>50.718000000000004</v>
       </c>
       <c r="G21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>950</v>
       </c>
@@ -2088,28 +2142,31 @@
         <v>50.845999999999997</v>
       </c>
       <c r="G22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H22">
         <v>12511</v>
       </c>
       <c r="I22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="N22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>979</v>
       </c>
@@ -2129,25 +2186,28 @@
         <v>54.274999999999999</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H23">
         <v>-999</v>
       </c>
       <c r="I23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K23" t="s">
         <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="N23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1008</v>
       </c>
@@ -2167,16 +2227,16 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K24" t="s">
         <v>26</v>
@@ -2185,10 +2245,10 @@
         <v>27</v>
       </c>
       <c r="M24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1011</v>
       </c>
@@ -2208,28 +2268,31 @@
         <v>43.664000000000001</v>
       </c>
       <c r="G25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H25">
         <v>2604</v>
       </c>
       <c r="I25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K25" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1090</v>
       </c>
@@ -2249,22 +2312,25 @@
         <v>51.164000000000001</v>
       </c>
       <c r="H26">
-        <v>-999</v>
+        <v>2653</v>
       </c>
       <c r="I26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K26" t="s">
         <v>17</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="N26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1095</v>
       </c>
@@ -2284,28 +2350,31 @@
         <v>48.564999999999998</v>
       </c>
       <c r="G27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H27">
         <v>839</v>
       </c>
       <c r="I27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K27" t="s">
         <v>17</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1096</v>
       </c>
@@ -2325,28 +2394,31 @@
         <v>47.786999999999999</v>
       </c>
       <c r="G28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H28">
         <v>1412</v>
       </c>
       <c r="I28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K28" t="s">
         <v>17</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="N28" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1290</v>
       </c>
@@ -2360,31 +2432,37 @@
         <v>54.1327</v>
       </c>
       <c r="E29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F29">
         <v>54.158999999999999</v>
       </c>
       <c r="G29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H29">
-        <v>-999</v>
+        <v>5313</v>
       </c>
       <c r="I29" t="s">
-        <v>130</v>
+        <v>291</v>
+      </c>
+      <c r="J29" t="s">
+        <v>290</v>
       </c>
       <c r="K29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="N29" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1303</v>
       </c>
@@ -2404,28 +2482,31 @@
         <v>50.908000000000001</v>
       </c>
       <c r="G30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J30" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N30" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1574</v>
       </c>
@@ -2445,25 +2526,28 @@
         <v>56.252000000000002</v>
       </c>
       <c r="G31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H31">
         <v>1111</v>
       </c>
       <c r="I31" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="M31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1720</v>
       </c>
@@ -2483,25 +2567,28 @@
         <v>52.155000000000001</v>
       </c>
       <c r="G32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="M32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="N32" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1721</v>
       </c>
@@ -2521,25 +2608,28 @@
         <v>59.429000000000002</v>
       </c>
       <c r="G33" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H33">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>144</v>
+        <v>292</v>
       </c>
       <c r="K33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="M33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N33" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1746</v>
       </c>
@@ -2559,28 +2649,31 @@
         <v>50.104999999999997</v>
       </c>
       <c r="G34" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H34">
         <v>684</v>
       </c>
       <c r="I34" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J34" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="K34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="M34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N34" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1781</v>
       </c>
@@ -2600,28 +2693,31 @@
         <v>42.667000000000002</v>
       </c>
       <c r="G35" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H35">
         <v>1073</v>
       </c>
       <c r="I35" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J35" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="K35" t="s">
         <v>17</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="M35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N35" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1806</v>
       </c>
@@ -2641,28 +2737,31 @@
         <v>50.436</v>
       </c>
       <c r="G36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="K36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="M36" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1812</v>
       </c>
@@ -2682,16 +2781,16 @@
         <v>63.442999999999998</v>
       </c>
       <c r="G37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K37" t="s">
         <v>26</v>
@@ -2700,10 +2799,10 @@
         <v>27</v>
       </c>
       <c r="M37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1821</v>
       </c>
@@ -2723,28 +2822,28 @@
         <v>63.058999999999997</v>
       </c>
       <c r="G38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="J38" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1842</v>
       </c>
@@ -2764,28 +2863,28 @@
         <v>58.143000000000001</v>
       </c>
       <c r="G39" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J39" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K39" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="M39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1863</v>
       </c>
@@ -2805,28 +2904,28 @@
         <v>58.16</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H40">
         <v>743.3</v>
       </c>
       <c r="I40" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J40" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K40" t="s">
+        <v>161</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M40" t="s">
         <v>166</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2063</v>
       </c>
@@ -2846,25 +2945,28 @@
         <v>55.643999999999998</v>
       </c>
       <c r="G41" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H41">
         <v>-999</v>
       </c>
       <c r="I41" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2071</v>
       </c>
@@ -2884,13 +2986,13 @@
         <v>61.057000000000002</v>
       </c>
       <c r="G42" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H42">
         <v>2718</v>
       </c>
       <c r="I42" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K42" t="s">
         <v>26</v>
@@ -2899,10 +3001,13 @@
         <v>27</v>
       </c>
       <c r="M42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2128</v>
       </c>
@@ -2922,28 +3027,31 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H43">
         <v>4240</v>
       </c>
       <c r="I43" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J43" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="K43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="M43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+      <c r="N43" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2132</v>
       </c>
@@ -2963,22 +3071,25 @@
         <v>65.683000000000007</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H44">
-        <v>-999</v>
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>293</v>
       </c>
       <c r="K44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2165</v>
       </c>
@@ -2992,31 +3103,34 @@
         <v>50.22336</v>
       </c>
       <c r="E45" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F45">
         <v>50.551000000000002</v>
       </c>
       <c r="G45" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H45">
         <v>1929</v>
       </c>
       <c r="J45" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K45" t="s">
         <v>17</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M45" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N45" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2170</v>
       </c>
@@ -3030,34 +3144,34 @@
         <v>51.698999999999998</v>
       </c>
       <c r="E46" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F46">
         <v>55.844999999999999</v>
       </c>
       <c r="G46" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H46">
         <v>4927.1000000000004</v>
       </c>
       <c r="I46" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J46" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="K46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M46" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2171</v>
       </c>
@@ -3071,34 +3185,34 @@
         <v>63.87473</v>
       </c>
       <c r="E47" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F47">
         <v>63.073</v>
       </c>
       <c r="G47" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H47">
         <v>4291.5</v>
       </c>
       <c r="I47" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J47" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="M47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2178</v>
       </c>
@@ -3118,16 +3232,16 @@
         <v>55.179000000000002</v>
       </c>
       <c r="G48" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H48">
         <v>1814</v>
       </c>
       <c r="I48" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="J48" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K48" t="s">
         <v>26</v>
@@ -3136,10 +3250,10 @@
         <v>27</v>
       </c>
       <c r="M48" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2183</v>
       </c>
@@ -3159,28 +3273,28 @@
         <v>55.52</v>
       </c>
       <c r="G49" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H49">
-        <v>-999</v>
+        <v>4777</v>
       </c>
       <c r="I49" t="s">
-        <v>203</v>
+        <v>280</v>
       </c>
       <c r="J49" t="s">
-        <v>204</v>
+        <v>281</v>
       </c>
       <c r="K49" t="s">
         <v>17</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="M49" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2185</v>
       </c>
@@ -3200,28 +3314,31 @@
         <v>49.021000000000001</v>
       </c>
       <c r="G50" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H50">
         <v>7121</v>
       </c>
       <c r="I50" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="J50" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="K50" t="s">
         <v>17</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="M50" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N50" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2209</v>
       </c>
@@ -3241,16 +3358,16 @@
         <v>51.658999999999999</v>
       </c>
       <c r="G51" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="J51" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="K51" t="s">
         <v>26</v>
@@ -3259,10 +3376,13 @@
         <v>27</v>
       </c>
       <c r="M51" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+      <c r="N51" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2232</v>
       </c>
@@ -3282,28 +3402,28 @@
         <v>48.945</v>
       </c>
       <c r="G52" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H52">
         <v>908</v>
       </c>
       <c r="I52" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="J52" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="K52" t="s">
         <v>17</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="M52" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2242</v>
       </c>
@@ -3323,28 +3443,28 @@
         <v>50.417000000000002</v>
       </c>
       <c r="G53" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H53">
         <v>663</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="J53" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="K53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="M53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2266</v>
       </c>
@@ -3364,13 +3484,13 @@
         <v>56.095999999999997</v>
       </c>
       <c r="G54" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="K54" t="s">
         <v>26</v>
@@ -3379,10 +3499,10 @@
         <v>27</v>
       </c>
       <c r="M54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2289</v>
       </c>
@@ -3396,34 +3516,37 @@
         <v>55.722000000000001</v>
       </c>
       <c r="E55" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F55">
         <v>55.807000000000002</v>
       </c>
       <c r="G55" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H55">
         <v>1131</v>
       </c>
       <c r="I55" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="J55" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="K55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="M55" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="N55" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2294</v>
       </c>
@@ -3443,28 +3566,28 @@
         <v>47.984999999999999</v>
       </c>
       <c r="G56" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="H56">
         <v>9013</v>
       </c>
       <c r="I56" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="J56" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="K56" t="s">
         <v>17</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="M56" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2308</v>
       </c>
@@ -3484,28 +3607,31 @@
         <v>56.402999999999999</v>
       </c>
       <c r="G57" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H57">
-        <v>-999</v>
+        <v>1243</v>
       </c>
       <c r="I57" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="J57" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="K57" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M57" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N57" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2321</v>
       </c>
@@ -3525,28 +3651,31 @@
         <v>54.218000000000004</v>
       </c>
       <c r="G58" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H58">
         <v>5672</v>
       </c>
       <c r="I58" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J58" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="K58" t="s">
         <v>17</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M58" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+      <c r="N58" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2322</v>
       </c>
@@ -3566,28 +3695,28 @@
         <v>52.75</v>
       </c>
       <c r="G59" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H59">
-        <v>-999</v>
+        <v>4870</v>
       </c>
       <c r="I59" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="J59" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="K59" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M59" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2323</v>
       </c>
@@ -3601,34 +3730,37 @@
         <v>57.582999999999998</v>
       </c>
       <c r="E60" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H60">
-        <v>2236.067</v>
+        <v>2236</v>
       </c>
       <c r="I60" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J60" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="K60" t="s">
         <v>17</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="M60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="N60" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2324</v>
       </c>
@@ -3648,28 +3780,31 @@
         <v>53.924999999999997</v>
       </c>
       <c r="G61" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="H61">
-        <v>-999</v>
+        <v>2430</v>
       </c>
       <c r="I61" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J61" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="K61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="N61" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>237</v>
       </c>
@@ -3680,7 +3815,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -3689,28 +3824,31 @@
         <v>57458</v>
       </c>
       <c r="G62" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="H62">
         <v>894</v>
       </c>
       <c r="I62" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J62" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="K62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="M62" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+      <c r="N62" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>254</v>
       </c>
@@ -3718,7 +3856,7 @@
         <v>99340</v>
       </c>
       <c r="C63" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D63">
         <v>49.462569999999999</v>
@@ -3730,28 +3868,31 @@
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H63">
         <v>1002</v>
       </c>
       <c r="I63" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J63" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="K63" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L63" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M63" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N63" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>313</v>
       </c>
@@ -3759,7 +3900,7 @@
         <v>98992</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D64">
         <v>51</v>
@@ -3771,25 +3912,28 @@
         <v>52.957000000000001</v>
       </c>
       <c r="G64" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H64">
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="K64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L64" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>382</v>
       </c>
@@ -3797,7 +3941,7 @@
         <v>98186</v>
       </c>
       <c r="C65" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D65">
         <v>45.465940000000003</v>
@@ -3809,25 +3953,28 @@
         <v>48.036999999999999</v>
       </c>
       <c r="G65" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="H65">
-        <v>-999</v>
+        <v>650</v>
       </c>
       <c r="I65" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="K65" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="L65" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M65" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>385</v>
       </c>
@@ -3835,7 +3982,7 @@
         <v>98184</v>
       </c>
       <c r="C66" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D66">
         <v>45.266280000000002</v>
@@ -3847,25 +3994,28 @@
         <v>48.037999999999997</v>
       </c>
       <c r="G66" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H66">
-        <v>-999</v>
+        <v>625</v>
       </c>
       <c r="I66" t="s">
-        <v>37</v>
+        <v>278</v>
+      </c>
+      <c r="J66" t="s">
+        <v>279</v>
       </c>
       <c r="K66" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="L66" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M66" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>408</v>
       </c>
@@ -3873,7 +4023,7 @@
         <v>97987</v>
       </c>
       <c r="C67" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D67">
         <v>50.181660000000001</v>
@@ -3885,28 +4035,28 @@
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H67">
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J67" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="K67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L67" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M67" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>405</v>
       </c>
@@ -3914,7 +4064,7 @@
         <v>97988</v>
       </c>
       <c r="C68" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D68">
         <v>50.18</v>
@@ -3926,25 +4076,25 @@
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="K68" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="L68" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="M68" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>922</v>
       </c>
@@ -3952,37 +4102,40 @@
         <v>96220</v>
       </c>
       <c r="C69" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D69">
         <v>48.61</v>
       </c>
       <c r="E69" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="K69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L69" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="N69" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1098</v>
       </c>
@@ -3990,7 +4143,7 @@
         <v>94209</v>
       </c>
       <c r="C70" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D70">
         <v>49.149000000000001</v>
@@ -4002,28 +4155,28 @@
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H70">
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J70" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="K70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L70" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M70" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>379</v>
       </c>
@@ -4031,7 +4184,7 @@
         <v>97851</v>
       </c>
       <c r="C71" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D71" s="5">
         <v>49225</v>
@@ -4043,22 +4196,25 @@
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="H71">
         <v>747</v>
       </c>
       <c r="I71" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="K71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="M71" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="N71" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TBC with proper rations in meters.
</commit_message>
<xml_diff>
--- a/data/data_vuv.xlsx
+++ b/data/data_vuv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="327">
   <si>
     <t>VarName1</t>
   </si>
@@ -1006,6 +1006,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 'Be II / 527 / 1.0 (3)'</t>
+  </si>
+  <si>
+    <t>STDSpeed</t>
   </si>
 </sst>
 </file>
@@ -1349,11 +1352,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H32" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="17280"/>
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="H46" sqref="H46"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -1372,7 +1375,7 @@
     <col min="12" max="12" width="45.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1421,8 +1424,11 @@
       <c r="P1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>66</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>76</v>
       </c>
@@ -1660,7 +1666,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>145</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>150</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>162</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>196</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>231</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>345</v>
       </c>
@@ -1960,7 +1966,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>652</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>655</v>
       </c>
@@ -2057,7 +2063,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>673</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>681</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1721</v>
       </c>
@@ -2974,7 +2980,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1746</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1781</v>
       </c>
@@ -3074,7 +3080,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1806</v>
       </c>
@@ -3124,7 +3130,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1812</v>
       </c>
@@ -3174,7 +3180,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1821</v>
       </c>
@@ -3224,7 +3230,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1842</v>
       </c>
@@ -3274,7 +3280,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1863</v>
       </c>
@@ -3324,7 +3330,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2063</v>
       </c>
@@ -3371,7 +3377,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2071</v>
       </c>
@@ -3418,7 +3424,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2128</v>
       </c>
@@ -3468,7 +3474,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2132</v>
       </c>
@@ -3515,7 +3521,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2165</v>
       </c>
@@ -3538,7 +3544,7 @@
         <v>180</v>
       </c>
       <c r="H45">
-        <v>1929</v>
+        <v>3831</v>
       </c>
       <c r="J45" t="s">
         <v>181</v>
@@ -3561,8 +3567,11 @@
       <c r="P45" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q45">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2170</v>
       </c>
@@ -3612,7 +3621,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2171</v>
       </c>
@@ -3661,8 +3670,12 @@
       <c r="P47" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q47">
+        <v>145.4</v>
+      </c>
+      <c r="R47" s="5"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2178</v>
       </c>

</xml_diff>

<commit_message>
Added the scale factors from pixel to meter.
</commit_message>
<xml_diff>
--- a/data/data_vuv.xlsx
+++ b/data/data_vuv.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="330">
   <si>
     <t>VarName1</t>
   </si>
@@ -942,9 +942,6 @@
     <t>(213, 428)</t>
   </si>
   <si>
-    <t>Sc_factor</t>
-  </si>
-  <si>
     <t>Many Ti UFOs during beams (50-56). biggest visble on op camps, more show up in spectroscopy.</t>
   </si>
   <si>
@@ -1009,12 +1006,27 @@
   </si>
   <si>
     <t>STDSpeed</t>
+  </si>
+  <si>
+    <t>TotRes</t>
+  </si>
+  <si>
+    <t>DistanceMeasured</t>
+  </si>
+  <si>
+    <t>ScFactor</t>
+  </si>
+  <si>
+    <t>OldScaledFactor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1053,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1072,6 +1084,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,11 +1365,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R78"/>
+  <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H32" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="17280"/>
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="S1" sqref="S1"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -1373,9 +1386,10 @@
     <col min="9" max="9" width="195.453125" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="12" max="12" width="45.1796875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1419,16 +1433,25 @@
         <v>288</v>
       </c>
       <c r="O1" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="P1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Q1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+      <c r="R1" t="s">
+        <v>329</v>
+      </c>
+      <c r="S1" t="s">
+        <v>328</v>
+      </c>
+      <c r="T1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1475,10 +1498,21 @@
         <v>127296</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+      <c r="R2" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S2">
+        <f>2.9091*R2</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T2">
+        <f>1.92*R2</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24</v>
       </c>
@@ -1519,10 +1553,21 @@
         <v>127296</v>
       </c>
       <c r="P3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R3" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S3">
+        <f>2.9091*R3</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T3">
+        <f>1.92*R3</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60</v>
       </c>
@@ -1566,10 +1611,21 @@
         <v>127296</v>
       </c>
       <c r="P4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R4" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S4">
+        <f>2.9091*R4</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T4">
+        <f>1.92*R4</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>66</v>
       </c>
@@ -1616,10 +1672,21 @@
         <v>127296</v>
       </c>
       <c r="P5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R5" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S5">
+        <f>2.9091*R5</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T5">
+        <f>1.92*R5</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>76</v>
       </c>
@@ -1663,10 +1730,21 @@
         <v>98304</v>
       </c>
       <c r="P6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+      <c r="R6">
+        <v>11.452999999999999</v>
+      </c>
+      <c r="S6">
+        <f>2.9091*R6</f>
+        <v>33.317922299999999</v>
+      </c>
+      <c r="T6">
+        <f>1.92*R6</f>
+        <v>21.989759999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>145</v>
       </c>
@@ -1713,10 +1791,21 @@
         <v>127296</v>
       </c>
       <c r="P7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R7" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S7">
+        <f>2.9091*R7</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T7">
+        <f>1.92*R7</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>150</v>
       </c>
@@ -1763,10 +1852,21 @@
         <v>127296</v>
       </c>
       <c r="P8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R8" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S8">
+        <f>2.9091*R8</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T8">
+        <f>1.92*R8</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>162</v>
       </c>
@@ -1813,10 +1913,21 @@
         <v>127296</v>
       </c>
       <c r="P9" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R9" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S9">
+        <f>2.9091*R9</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T9">
+        <f>1.92*R9</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>196</v>
       </c>
@@ -1863,10 +1974,21 @@
         <v>98304</v>
       </c>
       <c r="P10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+      <c r="R10">
+        <v>11.452999999999999</v>
+      </c>
+      <c r="S10">
+        <f>2.9091*R10</f>
+        <v>33.317922299999999</v>
+      </c>
+      <c r="T10">
+        <f>1.92*R10</f>
+        <v>21.989759999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>231</v>
       </c>
@@ -1913,10 +2035,21 @@
         <v>127296</v>
       </c>
       <c r="P11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R11" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S11">
+        <f>2.9091*R11</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T11">
+        <f>1.92*R11</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>345</v>
       </c>
@@ -1963,10 +2096,21 @@
         <v>131864</v>
       </c>
       <c r="P12" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R12">
+        <v>23.43</v>
+      </c>
+      <c r="S12">
+        <f>2.9091*R12</f>
+        <v>68.160212999999999</v>
+      </c>
+      <c r="T12">
+        <f>1.92*R12</f>
+        <v>44.985599999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>652</v>
       </c>
@@ -2010,10 +2154,21 @@
         <v>123410</v>
       </c>
       <c r="P13" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R13">
+        <v>33.33</v>
+      </c>
+      <c r="S13">
+        <f>2.9091*R13</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T13">
+        <f>1.92*R13</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>655</v>
       </c>
@@ -2060,10 +2215,21 @@
         <v>123410</v>
       </c>
       <c r="P14" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R14">
+        <v>33.33</v>
+      </c>
+      <c r="S14">
+        <f>2.9091*R14</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T14">
+        <f>1.92*R14</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>673</v>
       </c>
@@ -2107,10 +2273,21 @@
         <v>123410</v>
       </c>
       <c r="P15" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R15">
+        <v>33.33</v>
+      </c>
+      <c r="S15">
+        <f>2.9091*R15</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T15">
+        <f>1.92*R15</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>681</v>
       </c>
@@ -2154,10 +2331,21 @@
         <v>123410</v>
       </c>
       <c r="P16" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R16">
+        <v>33.33</v>
+      </c>
+      <c r="S16">
+        <f>2.9091*R16</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T16">
+        <f>1.92*R16</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>731</v>
       </c>
@@ -2204,10 +2392,21 @@
         <v>129560</v>
       </c>
       <c r="P17" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R17">
+        <v>26.05</v>
+      </c>
+      <c r="S17">
+        <f>2.9091*R17</f>
+        <v>75.782055</v>
+      </c>
+      <c r="T17">
+        <f>1.92*R17</f>
+        <v>50.015999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>737</v>
       </c>
@@ -2251,10 +2450,21 @@
         <v>262144</v>
       </c>
       <c r="P18" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R18">
+        <v>44.27</v>
+      </c>
+      <c r="S18">
+        <f>2.9091*R18</f>
+        <v>128.78585700000002</v>
+      </c>
+      <c r="T18">
+        <f>1.92*R18</f>
+        <v>84.998400000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>932</v>
       </c>
@@ -2301,10 +2511,21 @@
         <v>102400</v>
       </c>
       <c r="P19" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+      <c r="R19">
+        <v>16.48</v>
+      </c>
+      <c r="S19">
+        <f>2.9091*R19</f>
+        <v>47.941968000000003</v>
+      </c>
+      <c r="T19">
+        <f>1.92*R19</f>
+        <v>31.6416</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>944</v>
       </c>
@@ -2348,10 +2569,21 @@
         <v>133952</v>
       </c>
       <c r="P20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+      <c r="R20">
+        <v>27.08</v>
+      </c>
+      <c r="S20">
+        <f>2.9091*R20</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T20">
+        <f>1.92*R20</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>947</v>
       </c>
@@ -2395,10 +2627,21 @@
         <v>133952</v>
       </c>
       <c r="P21" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R21">
+        <v>27.08</v>
+      </c>
+      <c r="S21">
+        <f>2.9091*R21</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T21">
+        <f>1.92*R21</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>950</v>
       </c>
@@ -2445,10 +2688,21 @@
         <v>133952</v>
       </c>
       <c r="P22" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R22">
+        <v>27.08</v>
+      </c>
+      <c r="S22">
+        <f>2.9091*R22</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T22">
+        <f>1.92*R22</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>979</v>
       </c>
@@ -2492,10 +2746,21 @@
         <v>133952</v>
       </c>
       <c r="P23" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R23">
+        <v>27.08</v>
+      </c>
+      <c r="S23">
+        <f>2.9091*R23</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T23">
+        <f>1.92*R23</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1008</v>
       </c>
@@ -2542,10 +2807,21 @@
         <v>133952</v>
       </c>
       <c r="P24" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R24">
+        <v>27.08</v>
+      </c>
+      <c r="S24">
+        <f>2.9091*R24</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T24">
+        <f>1.92*R24</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1011</v>
       </c>
@@ -2592,10 +2868,21 @@
         <v>133952</v>
       </c>
       <c r="P25" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R25">
+        <v>27.08</v>
+      </c>
+      <c r="S25">
+        <f>2.9091*R25</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T25">
+        <f>1.92*R25</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1090</v>
       </c>
@@ -2636,10 +2923,21 @@
         <v>133952</v>
       </c>
       <c r="P26" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R26">
+        <v>27.08</v>
+      </c>
+      <c r="S26">
+        <f>2.9091*R26</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T26">
+        <f>1.92*R26</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1095</v>
       </c>
@@ -2686,10 +2984,21 @@
         <v>133952</v>
       </c>
       <c r="P27" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R27">
+        <v>27.08</v>
+      </c>
+      <c r="S27">
+        <f>2.9091*R27</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T27">
+        <f>1.92*R27</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1096</v>
       </c>
@@ -2736,10 +3045,21 @@
         <v>133952</v>
       </c>
       <c r="P28" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R28">
+        <v>27.08</v>
+      </c>
+      <c r="S28">
+        <f>2.9091*R28</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T28">
+        <f>1.92*R28</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1290</v>
       </c>
@@ -2786,10 +3106,21 @@
         <v>19840</v>
       </c>
       <c r="P29" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="R29">
+        <v>10.41</v>
+      </c>
+      <c r="S29">
+        <f>2.9091*R29</f>
+        <v>30.283731</v>
+      </c>
+      <c r="T29">
+        <f>1.92*R29</f>
+        <v>19.987199999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1303</v>
       </c>
@@ -2836,10 +3167,21 @@
         <v>130560</v>
       </c>
       <c r="P30" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R30">
+        <v>32.82</v>
+      </c>
+      <c r="S30">
+        <f>2.9091*R30</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T30">
+        <f>1.92*R30</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1574</v>
       </c>
@@ -2883,10 +3225,21 @@
         <v>130560</v>
       </c>
       <c r="P31" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R31">
+        <v>32.82</v>
+      </c>
+      <c r="S31">
+        <f>2.9091*R31</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T31">
+        <f>1.92*R31</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1720</v>
       </c>
@@ -2930,10 +3283,21 @@
         <v>98304</v>
       </c>
       <c r="P32" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+      <c r="R32">
+        <v>11.452999999999999</v>
+      </c>
+      <c r="S32">
+        <f>2.9091*R32</f>
+        <v>33.317922299999999</v>
+      </c>
+      <c r="T32">
+        <f>1.92*R32</f>
+        <v>21.989759999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1721</v>
       </c>
@@ -2977,10 +3341,21 @@
         <v>130560</v>
       </c>
       <c r="P33" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R33">
+        <v>32.82</v>
+      </c>
+      <c r="S33">
+        <f>2.9091*R33</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T33">
+        <f>1.92*R33</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1746</v>
       </c>
@@ -3027,10 +3402,21 @@
         <v>130560</v>
       </c>
       <c r="P34" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R34">
+        <v>32.82</v>
+      </c>
+      <c r="S34">
+        <f>2.9091*R34</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T34">
+        <f>1.92*R34</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1781</v>
       </c>
@@ -3077,10 +3463,21 @@
         <v>130560</v>
       </c>
       <c r="P35" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R35">
+        <v>32.82</v>
+      </c>
+      <c r="S35">
+        <f>2.9091*R35</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T35">
+        <f>1.92*R35</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1806</v>
       </c>
@@ -3127,10 +3524,21 @@
         <v>8160</v>
       </c>
       <c r="P36" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R36">
+        <v>6.68</v>
+      </c>
+      <c r="S36">
+        <f>2.9091*R36</f>
+        <v>19.432787999999999</v>
+      </c>
+      <c r="T36">
+        <f>1.92*R36</f>
+        <v>12.8256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1812</v>
       </c>
@@ -3177,10 +3585,21 @@
         <v>130560</v>
       </c>
       <c r="P37" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R37">
+        <v>32.82</v>
+      </c>
+      <c r="S37">
+        <f>2.9091*R37</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T37">
+        <f>1.92*R37</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1821</v>
       </c>
@@ -3227,10 +3646,21 @@
         <v>8160</v>
       </c>
       <c r="P38" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R38">
+        <v>6.68</v>
+      </c>
+      <c r="S38">
+        <f>2.9091*R38</f>
+        <v>19.432787999999999</v>
+      </c>
+      <c r="T38">
+        <f>1.92*R38</f>
+        <v>12.8256</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1842</v>
       </c>
@@ -3277,10 +3707,21 @@
         <v>130560</v>
       </c>
       <c r="P39" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R39">
+        <v>32.82</v>
+      </c>
+      <c r="S39">
+        <f>2.9091*R39</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T39">
+        <f>1.92*R39</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1863</v>
       </c>
@@ -3327,10 +3768,21 @@
         <v>130560</v>
       </c>
       <c r="P40" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R40">
+        <v>32.82</v>
+      </c>
+      <c r="S40">
+        <f>2.9091*R40</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T40">
+        <f>1.92*R40</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2063</v>
       </c>
@@ -3374,10 +3826,21 @@
         <v>127296</v>
       </c>
       <c r="P41" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R41" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S41">
+        <f>2.9091*R41</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T41">
+        <f>1.92*R41</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2071</v>
       </c>
@@ -3421,10 +3884,21 @@
         <v>98304</v>
       </c>
       <c r="P42" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+      <c r="R42">
+        <v>11.452999999999999</v>
+      </c>
+      <c r="S42">
+        <f>2.9091*R42</f>
+        <v>33.317922299999999</v>
+      </c>
+      <c r="T42">
+        <f>1.92*R42</f>
+        <v>21.989759999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2128</v>
       </c>
@@ -3471,10 +3945,21 @@
         <v>127296</v>
       </c>
       <c r="P43" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R43">
+        <v>29.68</v>
+      </c>
+      <c r="S43">
+        <f>2.9091*R43</f>
+        <v>86.342088000000004</v>
+      </c>
+      <c r="T43">
+        <f>1.92*R43</f>
+        <v>56.985599999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2132</v>
       </c>
@@ -3518,10 +4003,21 @@
         <v>127296</v>
       </c>
       <c r="P44" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R44">
+        <v>29.68</v>
+      </c>
+      <c r="S44">
+        <f>2.9091*R44</f>
+        <v>86.342088000000004</v>
+      </c>
+      <c r="T44">
+        <f>1.92*R44</f>
+        <v>56.985599999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2165</v>
       </c>
@@ -3565,13 +4061,24 @@
         <v>327680</v>
       </c>
       <c r="P45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q45">
         <v>1487</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R45" s="5">
+        <v>99.479200000000006</v>
+      </c>
+      <c r="S45">
+        <f>2.9091*R45</f>
+        <v>289.39494072000002</v>
+      </c>
+      <c r="T45">
+        <f>1.92*R45</f>
+        <v>191.00006400000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2170</v>
       </c>
@@ -3618,10 +4125,21 @@
         <v>116736</v>
       </c>
       <c r="P46" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+      <c r="R46">
+        <v>50</v>
+      </c>
+      <c r="S46">
+        <f>2.9091*R46</f>
+        <v>145.45500000000001</v>
+      </c>
+      <c r="T46">
+        <f>1.92*R46</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2171</v>
       </c>
@@ -3668,14 +4186,24 @@
         <v>327680</v>
       </c>
       <c r="P47" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q47">
         <v>145.4</v>
       </c>
-      <c r="R47" s="5"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R47" s="5">
+        <v>99.479200000000006</v>
+      </c>
+      <c r="S47">
+        <f>2.9091*R47</f>
+        <v>289.39494072000002</v>
+      </c>
+      <c r="T47">
+        <f>1.92*R47</f>
+        <v>191.00006400000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2178</v>
       </c>
@@ -3722,10 +4250,21 @@
         <v>127296</v>
       </c>
       <c r="P48" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R48" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S48">
+        <f>2.9091*R48</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T48">
+        <f>1.92*R48</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2183</v>
       </c>
@@ -3772,10 +4311,21 @@
         <v>127296</v>
       </c>
       <c r="P49" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R49" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S49">
+        <f>2.9091*R49</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T49">
+        <f>1.92*R49</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2185</v>
       </c>
@@ -3822,10 +4372,21 @@
         <v>127296</v>
       </c>
       <c r="P50" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R50" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S50">
+        <f>2.9091*R50</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T50">
+        <f>1.92*R50</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2209</v>
       </c>
@@ -3872,10 +4433,21 @@
         <v>127296</v>
       </c>
       <c r="P51" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R51" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S51">
+        <f>2.9091*R51</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T51">
+        <f>1.92*R51</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2232</v>
       </c>
@@ -3922,10 +4494,21 @@
         <v>127296</v>
       </c>
       <c r="P52" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R52" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S52">
+        <f>2.9091*R52</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T52">
+        <f>1.92*R52</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2242</v>
       </c>
@@ -3972,10 +4555,21 @@
         <v>123410</v>
       </c>
       <c r="P53" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R53" s="10">
+        <v>33.33</v>
+      </c>
+      <c r="S53">
+        <f>2.9091*R53</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T53">
+        <f>1.92*R53</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2266</v>
       </c>
@@ -4019,10 +4613,21 @@
         <v>133952</v>
       </c>
       <c r="P54" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R54">
+        <v>27.08</v>
+      </c>
+      <c r="S54">
+        <f>2.9091*R54</f>
+        <v>78.778427999999991</v>
+      </c>
+      <c r="T54">
+        <f>1.92*R54</f>
+        <v>51.993599999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2289</v>
       </c>
@@ -4069,10 +4674,21 @@
         <v>130560</v>
       </c>
       <c r="P55" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R55">
+        <v>32.82</v>
+      </c>
+      <c r="S55">
+        <f>2.9091*R55</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T55">
+        <f>1.92*R55</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2294</v>
       </c>
@@ -4119,10 +4735,21 @@
         <v>98304</v>
       </c>
       <c r="P56" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+      <c r="R56">
+        <v>11.452999999999999</v>
+      </c>
+      <c r="S56">
+        <f>2.9091*R56</f>
+        <v>33.317922299999999</v>
+      </c>
+      <c r="T56">
+        <f>1.92*R56</f>
+        <v>21.989759999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2308</v>
       </c>
@@ -4169,10 +4796,21 @@
         <v>127296</v>
       </c>
       <c r="P57" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R57" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S57">
+        <f>2.9091*R57</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T57">
+        <f>1.92*R57</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2321</v>
       </c>
@@ -4219,10 +4857,21 @@
         <v>127296</v>
       </c>
       <c r="P58" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R58" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S58">
+        <f>2.9091*R58</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T58">
+        <f>1.92*R58</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2322</v>
       </c>
@@ -4269,10 +4918,21 @@
         <v>127296</v>
       </c>
       <c r="P59" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R59" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S59">
+        <f>2.9091*R59</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T59">
+        <f>1.92*R59</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2323</v>
       </c>
@@ -4319,10 +4979,21 @@
         <v>19200</v>
       </c>
       <c r="P60" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="R60" s="10">
+        <v>10.41</v>
+      </c>
+      <c r="S60">
+        <f>2.9091*R60</f>
+        <v>30.283731</v>
+      </c>
+      <c r="T60">
+        <f>1.92*R60</f>
+        <v>19.987199999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2324</v>
       </c>
@@ -4369,10 +5040,21 @@
         <v>127296</v>
       </c>
       <c r="P61" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R61" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S61">
+        <f>2.9091*R61</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T61">
+        <f>1.92*R61</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>237</v>
       </c>
@@ -4419,10 +5101,21 @@
         <v>127296</v>
       </c>
       <c r="P62" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R62" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S62">
+        <f>2.9091*R62</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T62">
+        <f>1.92*R62</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>254</v>
       </c>
@@ -4469,10 +5162,21 @@
         <v>127296</v>
       </c>
       <c r="P63" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R63" s="10">
+        <v>33.854199999999999</v>
+      </c>
+      <c r="S63">
+        <f>2.9091*R63</f>
+        <v>98.48525321999999</v>
+      </c>
+      <c r="T63">
+        <f>1.92*R63</f>
+        <v>65.000063999999995</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>313</v>
       </c>
@@ -4516,10 +5220,21 @@
         <v>31824</v>
       </c>
       <c r="P64" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R64" s="10">
+        <v>10.414999999999999</v>
+      </c>
+      <c r="S64">
+        <f>2.9091*R64</f>
+        <v>30.298276499999997</v>
+      </c>
+      <c r="T64">
+        <f>1.92*R64</f>
+        <v>19.996799999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>382</v>
       </c>
@@ -4563,10 +5278,21 @@
         <v>131864</v>
       </c>
       <c r="P65" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+      <c r="R65">
+        <v>23.43</v>
+      </c>
+      <c r="S65">
+        <f>2.9091*R65</f>
+        <v>68.160212999999999</v>
+      </c>
+      <c r="T65">
+        <f>1.92*R65</f>
+        <v>44.985599999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>385</v>
       </c>
@@ -4613,10 +5339,21 @@
         <v>131864</v>
       </c>
       <c r="P66" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+      <c r="R66">
+        <v>23.43</v>
+      </c>
+      <c r="S66">
+        <f>2.9091*R66</f>
+        <v>68.160212999999999</v>
+      </c>
+      <c r="T66">
+        <f>1.92*R66</f>
+        <v>44.985599999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>408</v>
       </c>
@@ -4663,10 +5400,21 @@
         <v>123410</v>
       </c>
       <c r="P67" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+      <c r="R67">
+        <v>33.33</v>
+      </c>
+      <c r="S67">
+        <f>2.9091*R67</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T67">
+        <f>1.92*R67</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>405</v>
       </c>
@@ -4710,10 +5458,21 @@
         <v>123410</v>
       </c>
       <c r="P68" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+      <c r="R68">
+        <v>33.33</v>
+      </c>
+      <c r="S68">
+        <f>2.9091*R68</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T68">
+        <f>1.92*R68</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>922</v>
       </c>
@@ -4757,10 +5516,21 @@
         <v>21120</v>
       </c>
       <c r="P69" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="R69">
+        <v>10.41</v>
+      </c>
+      <c r="S69">
+        <f>2.9091*R69</f>
+        <v>30.283731</v>
+      </c>
+      <c r="T69">
+        <f>1.92*R69</f>
+        <v>19.987199999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1098</v>
       </c>
@@ -4804,10 +5574,21 @@
         <v>143936</v>
       </c>
       <c r="P70" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+      <c r="R70">
+        <v>20.83</v>
+      </c>
+      <c r="S70">
+        <f>2.9091*R70</f>
+        <v>60.596552999999993</v>
+      </c>
+      <c r="T70">
+        <f>1.92*R70</f>
+        <v>39.993599999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>379</v>
       </c>
@@ -4851,10 +5632,21 @@
         <v>123410</v>
       </c>
       <c r="P71" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R71">
+        <v>33.33</v>
+      </c>
+      <c r="S71">
+        <f>2.9091*R71</f>
+        <v>96.960302999999996</v>
+      </c>
+      <c r="T71">
+        <f>1.92*R71</f>
+        <v>63.993599999999994</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1739</v>
       </c>
@@ -4898,10 +5690,21 @@
         <v>130560</v>
       </c>
       <c r="P72" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R72">
+        <v>32.82</v>
+      </c>
+      <c r="S72">
+        <f>2.9091*R72</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T72">
+        <f>1.92*R72</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1568</v>
       </c>
@@ -4945,10 +5748,21 @@
         <v>130560</v>
       </c>
       <c r="P73" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="R73">
+        <v>32.82</v>
+      </c>
+      <c r="S73">
+        <f>2.9091*R73</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T73">
+        <f>1.92*R73</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1730</v>
       </c>
@@ -4995,10 +5809,21 @@
         <v>130560</v>
       </c>
       <c r="P74" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R74">
+        <v>32.82</v>
+      </c>
+      <c r="S74">
+        <f>2.9091*R74</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T74">
+        <f>1.92*R74</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1733</v>
       </c>
@@ -5045,10 +5870,21 @@
         <v>130560</v>
       </c>
       <c r="P75" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R75">
+        <v>32.82</v>
+      </c>
+      <c r="S75">
+        <f>2.9091*R75</f>
+        <v>95.476662000000005</v>
+      </c>
+      <c r="T75">
+        <f>1.92*R75</f>
+        <v>63.014399999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1593</v>
       </c>
@@ -5068,16 +5904,16 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H76">
         <v>0</v>
       </c>
       <c r="I76" t="s">
+        <v>305</v>
+      </c>
+      <c r="J76" t="s">
         <v>306</v>
-      </c>
-      <c r="J76" t="s">
-        <v>307</v>
       </c>
       <c r="K76" t="s">
         <v>53</v>
@@ -5095,10 +5931,21 @@
         <v>153600</v>
       </c>
       <c r="P76" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R76">
+        <v>41.6</v>
+      </c>
+      <c r="S76">
+        <f>2.9091*R76</f>
+        <v>121.01856000000001</v>
+      </c>
+      <c r="T76">
+        <f>1.92*R76</f>
+        <v>79.872</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1599</v>
       </c>
@@ -5118,16 +5965,16 @@
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H77">
         <v>0</v>
       </c>
       <c r="I77" t="s">
+        <v>308</v>
+      </c>
+      <c r="J77" t="s">
         <v>309</v>
-      </c>
-      <c r="J77" t="s">
-        <v>310</v>
       </c>
       <c r="K77" t="s">
         <v>53</v>
@@ -5145,10 +5992,21 @@
         <v>153600</v>
       </c>
       <c r="P77" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="R77">
+        <v>41.6</v>
+      </c>
+      <c r="S77">
+        <f>2.9091*R77</f>
+        <v>121.01856000000001</v>
+      </c>
+      <c r="T77">
+        <f>1.92*R77</f>
+        <v>79.872</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1596</v>
       </c>
@@ -5168,16 +6026,16 @@
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H78">
         <v>-999</v>
       </c>
       <c r="I78" t="s">
+        <v>311</v>
+      </c>
+      <c r="J78" t="s">
         <v>312</v>
-      </c>
-      <c r="J78" t="s">
-        <v>313</v>
       </c>
       <c r="K78" t="s">
         <v>53</v>
@@ -5195,7 +6053,18 @@
         <v>153600</v>
       </c>
       <c r="P78" t="s">
-        <v>325</v>
+        <v>324</v>
+      </c>
+      <c r="R78">
+        <v>41.6</v>
+      </c>
+      <c r="S78">
+        <f>2.9091*R78</f>
+        <v>121.01856000000001</v>
+      </c>
+      <c r="T78">
+        <f>1.92*R78</f>
+        <v>79.872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scale factor from the ACF model.
</commit_message>
<xml_diff>
--- a/data/data_vuv.xlsx
+++ b/data/data_vuv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="332">
   <si>
     <t>VarName1</t>
   </si>
@@ -1018,6 +1018,12 @@
   </si>
   <si>
     <t>OldScaledFactor</t>
+  </si>
+  <si>
+    <t>DistanceACF</t>
+  </si>
+  <si>
+    <t>ACFFactor</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1031,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1084,7 +1090,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1365,11 +1371,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T78"/>
+  <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="17280"/>
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="D7" sqref="D7"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -1389,7 +1395,7 @@
     <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1450,8 +1456,14 @@
       <c r="T1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U1" t="s">
+        <v>330</v>
+      </c>
+      <c r="V1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1511,8 +1523,15 @@
         <f>1.92*R2</f>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U2" s="5">
+        <v>55.604199999999999</v>
+      </c>
+      <c r="V2">
+        <f>U2*1.51</f>
+        <v>83.962341999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24</v>
       </c>
@@ -1559,15 +1578,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S3">
-        <f>2.9091*R3</f>
+        <f t="shared" ref="S3:S33" si="0">2.9091*R3</f>
         <v>98.48525321999999</v>
       </c>
       <c r="T3">
-        <f>1.92*R3</f>
+        <f t="shared" ref="T3:T33" si="1">1.92*R3</f>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U3" s="5">
+        <v>53.1233</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V66" si="2">U3*1.51</f>
+        <v>80.216183000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60</v>
       </c>
@@ -1617,15 +1643,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S4">
-        <f>2.9091*R4</f>
+        <f t="shared" si="0"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T4">
-        <f>1.92*R4</f>
+        <f t="shared" si="1"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U4" s="5">
+        <v>57.2</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="2"/>
+        <v>86.372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>66</v>
       </c>
@@ -1678,175 +1711,196 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S5">
-        <f>2.9091*R5</f>
+        <f t="shared" si="0"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T5">
-        <f>1.92*R5</f>
+        <f t="shared" si="1"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U5">
+        <v>65</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>98.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>76</v>
+        <v>1290</v>
       </c>
       <c r="B6">
-        <v>99868</v>
+        <v>104462</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>48.709119999999999</v>
+        <v>54.1327</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>54.158999999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="H6">
-        <v>3794.73</v>
+        <v>5313</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>291</v>
+      </c>
+      <c r="J6" t="s">
+        <v>290</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="N6" t="s">
         <v>287</v>
       </c>
       <c r="O6">
-        <v>98304</v>
+        <v>19840</v>
       </c>
       <c r="P6" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="R6">
-        <v>11.452999999999999</v>
+        <v>10.41</v>
       </c>
       <c r="S6">
         <f>2.9091*R6</f>
-        <v>33.317922299999999</v>
+        <v>30.283731</v>
       </c>
       <c r="T6">
         <f>1.92*R6</f>
-        <v>21.989759999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+        <v>19.987199999999998</v>
+      </c>
+      <c r="U6">
+        <v>20</v>
+      </c>
+      <c r="V6">
+        <f>U6*1.51</f>
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="B7">
-        <v>99724</v>
+        <v>99868</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>53.616300000000003</v>
+        <v>48.709119999999999</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F7">
-        <v>61.036999999999999</v>
+        <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>3794.73</v>
       </c>
       <c r="I7" t="s">
-        <v>283</v>
-      </c>
-      <c r="J7" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="N7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O7">
-        <v>127296</v>
+        <v>98304</v>
       </c>
       <c r="P7" t="s">
-        <v>314</v>
-      </c>
-      <c r="R7" s="10">
-        <v>33.854199999999999</v>
+        <v>315</v>
+      </c>
+      <c r="R7">
+        <v>11.452999999999999</v>
       </c>
       <c r="S7">
-        <f>2.9091*R7</f>
-        <v>98.48525321999999</v>
+        <f t="shared" si="0"/>
+        <v>33.317922299999999</v>
       </c>
       <c r="T7">
-        <f>1.92*R7</f>
-        <v>65.000063999999995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>21.989759999999997</v>
+      </c>
+      <c r="U7" s="5">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>78.394216999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B8">
-        <v>99697</v>
+        <v>99724</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8">
-        <v>53.51</v>
+        <v>53.616300000000003</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8">
-        <v>58.750999999999998</v>
+        <v>61.036999999999999</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H8">
-        <v>1409</v>
+        <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>283</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M8" t="s">
         <v>40</v>
       </c>
       <c r="N8" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O8">
         <v>127296</v>
@@ -1857,51 +1911,58 @@
       <c r="R8" s="10">
         <v>33.854199999999999</v>
       </c>
-      <c r="S8">
-        <f>2.9091*R8</f>
-        <v>98.48525321999999</v>
+      <c r="S8" t="e">
+        <f>2.9091*T7R7</f>
+        <v>#NAME?</v>
       </c>
       <c r="T8">
-        <f>1.92*R8</f>
+        <f t="shared" si="1"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" s="5">
+        <v>56.804900000000004</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>85.775399000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B9">
-        <v>99640</v>
+        <v>99697</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>46.2</v>
+        <v>53.51</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9">
-        <v>46.377000000000002</v>
+        <v>58.750999999999998</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H9">
-        <v>3635</v>
+        <v>1409</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="M9" t="s">
         <v>40</v>
@@ -1919,294 +1980,329 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S9">
-        <f>2.9091*R9</f>
+        <f t="shared" si="0"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T9">
-        <f>1.92*R9</f>
+        <f t="shared" si="1"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" s="5">
+        <v>58.6905</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>88.622654999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B10">
-        <v>99541</v>
+        <v>99640</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10">
-        <v>50.166400000000003</v>
+        <v>46.2</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F10">
-        <v>50.892000000000003</v>
+        <v>46.377000000000002</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>3635</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K10" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="N10" t="s">
         <v>287</v>
       </c>
       <c r="O10">
-        <v>98304</v>
+        <v>127296</v>
       </c>
       <c r="P10" t="s">
-        <v>315</v>
-      </c>
-      <c r="R10">
-        <v>11.452999999999999</v>
+        <v>314</v>
+      </c>
+      <c r="R10" s="10">
+        <v>33.854199999999999</v>
       </c>
       <c r="S10">
-        <f>2.9091*R10</f>
-        <v>33.317922299999999</v>
+        <f t="shared" si="0"/>
+        <v>98.48525321999999</v>
       </c>
       <c r="T10">
-        <f>1.92*R10</f>
-        <v>21.989759999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>65.000063999999995</v>
+      </c>
+      <c r="U10">
+        <v>65</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>98.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="B11">
-        <v>99453</v>
+        <v>99541</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11">
-        <v>47.328919999999997</v>
+        <v>50.166400000000003</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F11">
-        <v>47.408999999999999</v>
+        <v>50.892000000000003</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H11">
-        <v>3535</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="M11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N11" t="s">
         <v>287</v>
       </c>
       <c r="O11">
-        <v>127296</v>
+        <v>98304</v>
       </c>
       <c r="P11" t="s">
-        <v>314</v>
-      </c>
-      <c r="R11" s="10">
-        <v>33.854199999999999</v>
+        <v>315</v>
+      </c>
+      <c r="R11">
+        <v>11.452999999999999</v>
       </c>
       <c r="S11">
-        <f>2.9091*R11</f>
-        <v>98.48525321999999</v>
+        <f t="shared" si="0"/>
+        <v>33.317922299999999</v>
       </c>
       <c r="T11">
-        <f>1.92*R11</f>
-        <v>65.000063999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>21.989759999999997</v>
+      </c>
+      <c r="U11" s="5">
+        <v>55.308599999999998</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>83.515985999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>345</v>
+        <v>231</v>
       </c>
       <c r="B12">
-        <v>98786</v>
+        <v>99453</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12">
-        <v>57.53</v>
+        <v>47.328919999999997</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12">
-        <v>57.530999999999999</v>
+        <v>47.408999999999999</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H12">
-        <v>6134.5</v>
+        <v>3535</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="M12" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="N12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O12">
-        <v>131864</v>
+        <v>127296</v>
       </c>
       <c r="P12" t="s">
         <v>314</v>
       </c>
-      <c r="R12">
-        <v>23.43</v>
+      <c r="R12" s="10">
+        <v>33.854199999999999</v>
       </c>
       <c r="S12">
-        <f>2.9091*R12</f>
-        <v>68.160212999999999</v>
+        <f t="shared" si="0"/>
+        <v>98.48525321999999</v>
       </c>
       <c r="T12">
-        <f>1.92*R12</f>
-        <v>44.985599999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>65.000063999999995</v>
+      </c>
+      <c r="U12" s="5">
+        <v>46.5</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="2"/>
+        <v>70.215000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>652</v>
+        <v>345</v>
       </c>
       <c r="B13">
-        <v>97045</v>
+        <v>98786</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13">
-        <v>48.504959999999997</v>
+        <v>57.53</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>66</v>
+        <v>57.530999999999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
       </c>
       <c r="H13">
-        <v>2096</v>
+        <v>6134.5</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M13" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="N13" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O13">
-        <v>123410</v>
+        <v>131864</v>
       </c>
       <c r="P13" t="s">
         <v>314</v>
       </c>
       <c r="R13">
-        <v>33.33</v>
+        <v>23.43</v>
       </c>
       <c r="S13">
-        <f>2.9091*R13</f>
-        <v>96.960302999999996</v>
+        <f t="shared" si="0"/>
+        <v>68.160212999999999</v>
       </c>
       <c r="T13">
-        <f>1.92*R13</f>
-        <v>63.993599999999994</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>44.985599999999998</v>
+      </c>
+      <c r="U13" s="5">
+        <v>49.5</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="2"/>
+        <v>74.745000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B14">
-        <v>97044</v>
+        <v>97045</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
       <c r="D14">
-        <v>42.346820000000001</v>
+        <v>48.504959999999997</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14">
-        <v>42.408000000000001</v>
-      </c>
-      <c r="G14" t="s">
-        <v>71</v>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H14">
-        <v>3928</v>
+        <v>2096</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" t="s">
-        <v>284</v>
+        <v>67</v>
       </c>
       <c r="K14" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M14" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="N14" t="s">
         <v>287</v>
@@ -2221,50 +2317,60 @@
         <v>33.33</v>
       </c>
       <c r="S14">
-        <f>2.9091*R14</f>
+        <f t="shared" si="0"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T14">
-        <f>1.92*R14</f>
+        <f t="shared" si="1"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U14" s="5">
+        <v>57.849299999999999</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="2"/>
+        <v>87.352442999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>673</v>
+        <v>655</v>
       </c>
       <c r="B15">
-        <v>96990</v>
+        <v>97044</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
       <c r="D15">
-        <v>60.214770000000001</v>
+        <v>42.346820000000001</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>60.258000000000003</v>
+        <v>42.408000000000001</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H15">
-        <v>3259</v>
+        <v>3928</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="J15" t="s">
+        <v>284</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="N15" t="s">
         <v>287</v>
@@ -2279,50 +2385,57 @@
         <v>33.33</v>
       </c>
       <c r="S15">
-        <f>2.9091*R15</f>
+        <f t="shared" si="0"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T15">
-        <f>1.92*R15</f>
+        <f t="shared" si="1"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U15" s="5">
+        <v>42.631599999999999</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="2"/>
+        <v>64.373716000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="B16">
-        <v>96956</v>
+        <v>96990</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
       <c r="D16">
-        <v>55.571899999999999</v>
+        <v>60.214770000000001</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="F16">
-        <v>55.588000000000001</v>
+        <v>60.258000000000003</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H16">
-        <v>837</v>
+        <v>3259</v>
       </c>
       <c r="I16" t="s">
-        <v>285</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N16" t="s">
         <v>287</v>
@@ -2337,353 +2450,392 @@
         <v>33.33</v>
       </c>
       <c r="S16">
-        <f>2.9091*R16</f>
+        <f t="shared" si="0"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T16">
-        <f>1.92*R16</f>
+        <f t="shared" si="1"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U16" s="5">
+        <v>67</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="2"/>
+        <v>101.17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>731</v>
+        <v>681</v>
       </c>
       <c r="B17">
-        <v>96818</v>
+        <v>96956</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17">
-        <v>43.74</v>
+        <v>55.571899999999999</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="F17">
-        <v>43.744</v>
+        <v>55.588000000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H17">
-        <v>1596</v>
+        <v>837</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
-      </c>
-      <c r="J17" t="s">
-        <v>82</v>
+        <v>285</v>
       </c>
       <c r="K17" t="s">
         <v>17</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="M17" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="N17" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O17">
-        <v>129560</v>
+        <v>123410</v>
       </c>
       <c r="P17" t="s">
         <v>314</v>
       </c>
       <c r="R17">
-        <v>26.05</v>
+        <v>33.33</v>
       </c>
       <c r="S17">
-        <f>2.9091*R17</f>
-        <v>75.782055</v>
+        <f t="shared" si="0"/>
+        <v>96.960302999999996</v>
       </c>
       <c r="T17">
-        <f>1.92*R17</f>
-        <v>50.015999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>63.993599999999994</v>
+      </c>
+      <c r="U17" s="5">
+        <v>53</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="2"/>
+        <v>80.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="B18">
-        <v>96815</v>
+        <v>96818</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18">
-        <v>43.82</v>
+        <v>43.74</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>43.744</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H18">
-        <v>-999</v>
+        <v>1596</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
       </c>
       <c r="K18" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="N18" t="s">
         <v>289</v>
       </c>
       <c r="O18">
-        <v>262144</v>
+        <v>129560</v>
       </c>
       <c r="P18" t="s">
         <v>314</v>
       </c>
       <c r="R18">
-        <v>44.27</v>
+        <v>26.05</v>
       </c>
       <c r="S18">
-        <f>2.9091*R18</f>
-        <v>128.78585700000002</v>
+        <f t="shared" si="0"/>
+        <v>75.782055</v>
       </c>
       <c r="T18">
-        <f>1.92*R18</f>
-        <v>84.998400000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>50.015999999999998</v>
+      </c>
+      <c r="U18" s="5">
+        <v>45.5</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="2"/>
+        <v>68.704999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>932</v>
+        <v>737</v>
       </c>
       <c r="B19">
-        <v>96125</v>
+        <v>96815</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
       <c r="D19">
-        <v>63.044220000000003</v>
+        <v>43.82</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F19">
-        <v>63.055999999999997</v>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H19">
-        <v>3810</v>
+        <v>-999</v>
       </c>
       <c r="I19" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K19" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="M19" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="N19" t="s">
         <v>289</v>
       </c>
       <c r="O19">
-        <v>102400</v>
+        <v>262144</v>
       </c>
       <c r="P19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="R19">
-        <v>16.48</v>
+        <v>44.27</v>
       </c>
       <c r="S19">
-        <f>2.9091*R19</f>
-        <v>47.941968000000003</v>
+        <f t="shared" si="0"/>
+        <v>128.78585700000002</v>
       </c>
       <c r="T19">
-        <f>1.92*R19</f>
-        <v>31.6416</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>84.998400000000004</v>
+      </c>
+      <c r="U19">
+        <v>85</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="2"/>
+        <v>128.35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>944</v>
+        <v>932</v>
       </c>
       <c r="B20">
-        <v>96067</v>
+        <v>96125</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20">
-        <v>49.969670000000001</v>
+        <v>63.044220000000003</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F20">
-        <v>50.985999999999997</v>
+        <v>63.055999999999997</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>3810</v>
       </c>
       <c r="I20" t="s">
-        <v>286</v>
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
+        <v>90</v>
       </c>
       <c r="K20" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="N20" t="s">
         <v>289</v>
       </c>
       <c r="O20">
-        <v>133952</v>
+        <v>102400</v>
       </c>
       <c r="P20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R20">
-        <v>27.08</v>
+        <v>16.48</v>
       </c>
       <c r="S20">
-        <f>2.9091*R20</f>
-        <v>78.778427999999991</v>
+        <f t="shared" si="0"/>
+        <v>47.941968000000003</v>
       </c>
       <c r="T20">
-        <f>1.92*R20</f>
-        <v>51.993599999999994</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>31.6416</v>
+      </c>
+      <c r="U20" s="5">
+        <v>51.627899999999997</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="2"/>
+        <v>77.958129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="B21">
-        <v>96045</v>
+        <v>96067</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
       <c r="D21">
-        <v>44.216419999999999</v>
+        <v>49.969670000000001</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
       <c r="F21">
-        <v>50.718000000000004</v>
+        <v>50.985999999999997</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>97</v>
-      </c>
-      <c r="J21" t="s">
-        <v>98</v>
+        <v>286</v>
       </c>
       <c r="K21" t="s">
         <v>53</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M21" t="s">
         <v>23</v>
       </c>
+      <c r="N21" t="s">
+        <v>289</v>
+      </c>
       <c r="O21">
         <v>133952</v>
       </c>
       <c r="P21" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="R21">
         <v>27.08</v>
       </c>
       <c r="S21">
-        <f>2.9091*R21</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T21">
-        <f>1.92*R21</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U21" s="5">
+        <v>52</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="2"/>
+        <v>78.52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="B22">
-        <v>96040</v>
+        <v>96045</v>
       </c>
       <c r="C22">
         <v>5</v>
       </c>
       <c r="D22">
-        <v>50.219580000000001</v>
+        <v>44.216419999999999</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
       </c>
       <c r="F22">
-        <v>50.845999999999997</v>
+        <v>50.718000000000004</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H22">
-        <v>12511</v>
+        <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K22" t="s">
         <v>53</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M22" t="s">
         <v>23</v>
       </c>
-      <c r="N22" t="s">
-        <v>289</v>
-      </c>
       <c r="O22">
         <v>133952</v>
       </c>
@@ -2694,53 +2846,63 @@
         <v>27.08</v>
       </c>
       <c r="S22">
-        <f>2.9091*R22</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T22">
-        <f>1.92*R22</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U22" s="5">
+        <v>58.444400000000002</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="2"/>
+        <v>88.251044000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>979</v>
+        <v>950</v>
       </c>
       <c r="B23">
-        <v>96002</v>
+        <v>96040</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
       <c r="D23">
-        <v>54.047229999999999</v>
+        <v>50.219580000000001</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
       </c>
       <c r="F23">
-        <v>54.274999999999999</v>
+        <v>50.845999999999997</v>
       </c>
       <c r="G23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H23">
-        <v>-999</v>
+        <v>12511</v>
       </c>
       <c r="I23" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="J23" t="s">
+        <v>102</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M23" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="N23" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O23">
         <v>133952</v>
@@ -2752,56 +2914,60 @@
         <v>27.08</v>
       </c>
       <c r="S23">
-        <f>2.9091*R23</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T23">
-        <f>1.92*R23</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U23" s="5">
+        <v>53.829300000000003</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="2"/>
+        <v>81.282243000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>1008</v>
+        <v>979</v>
       </c>
       <c r="B24">
-        <v>95716</v>
+        <v>96002</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="D24">
-        <v>45.122570000000003</v>
+        <v>54.047229999999999</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>54.274999999999999</v>
       </c>
       <c r="G24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>-999</v>
       </c>
       <c r="I24" t="s">
-        <v>108</v>
-      </c>
-      <c r="J24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K24" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="M24" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="N24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O24">
         <v>133952</v>
@@ -2813,56 +2979,63 @@
         <v>27.08</v>
       </c>
       <c r="S24">
-        <f>2.9091*R24</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T24">
-        <f>1.92*R24</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U24" s="5">
+        <v>86</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="2"/>
+        <v>129.86000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="B25">
-        <v>95713</v>
+        <v>95716</v>
       </c>
       <c r="C25">
         <v>5</v>
       </c>
       <c r="D25">
-        <v>43.338999999999999</v>
+        <v>45.122570000000003</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
       <c r="F25">
-        <v>43.664000000000001</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H25">
-        <v>2604</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K25" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="M25" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N25" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O25">
         <v>133952</v>
@@ -2874,47 +3047,60 @@
         <v>27.08</v>
       </c>
       <c r="S25">
-        <f>2.9091*R25</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T25">
-        <f>1.92*R25</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U25" s="5">
+        <v>63.087499999999999</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="2"/>
+        <v>95.262124999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>1090</v>
+        <v>1011</v>
       </c>
       <c r="B26">
-        <v>95374</v>
+        <v>95713</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26">
-        <v>50.819009999999999</v>
+        <v>43.338999999999999</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26">
-        <v>51.164000000000001</v>
+        <v>43.664000000000001</v>
+      </c>
+      <c r="G26" t="s">
+        <v>111</v>
       </c>
       <c r="H26">
-        <v>2653</v>
+        <v>2604</v>
       </c>
       <c r="I26" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="J26" t="s">
+        <v>113</v>
       </c>
       <c r="K26" t="s">
         <v>17</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M26" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="N26" t="s">
         <v>287</v>
@@ -2929,56 +3115,57 @@
         <v>27.08</v>
       </c>
       <c r="S26">
-        <f>2.9091*R26</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T26">
-        <f>1.92*R26</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U26" s="5">
+        <v>52.882399999999997</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="2"/>
+        <v>79.852423999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>1095</v>
+        <v>1090</v>
       </c>
       <c r="B27">
-        <v>95319</v>
+        <v>95374</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27">
-        <v>48.361040000000003</v>
+        <v>50.819009999999999</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
       <c r="F27">
-        <v>48.564999999999998</v>
-      </c>
-      <c r="G27" t="s">
-        <v>117</v>
+        <v>51.164000000000001</v>
       </c>
       <c r="H27">
-        <v>839</v>
+        <v>2653</v>
       </c>
       <c r="I27" t="s">
-        <v>118</v>
-      </c>
-      <c r="J27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K27" t="s">
         <v>17</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M27" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N27" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O27">
         <v>133952</v>
@@ -2990,53 +3177,60 @@
         <v>27.08</v>
       </c>
       <c r="S27">
-        <f>2.9091*R27</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T27">
-        <f>1.92*R27</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U27" s="5">
+        <v>60.428600000000003</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="2"/>
+        <v>91.247185999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B28">
-        <v>95314</v>
+        <v>95319</v>
       </c>
       <c r="C28">
         <v>5</v>
       </c>
       <c r="D28">
-        <v>47.013210000000001</v>
+        <v>48.361040000000003</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
       </c>
       <c r="F28">
-        <v>47.786999999999999</v>
+        <v>48.564999999999998</v>
       </c>
       <c r="G28" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H28">
-        <v>1412</v>
+        <v>839</v>
       </c>
       <c r="I28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K28" t="s">
         <v>17</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M28" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="N28" t="s">
         <v>289</v>
@@ -3051,76 +3245,90 @@
         <v>27.08</v>
       </c>
       <c r="S28">
-        <f>2.9091*R28</f>
+        <f t="shared" si="0"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T28">
-        <f>1.92*R28</f>
+        <f t="shared" si="1"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U28">
+        <v>52</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="2"/>
+        <v>78.52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>1290</v>
+        <v>1096</v>
       </c>
       <c r="B29">
-        <v>104462</v>
+        <v>95314</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29">
-        <v>54.1327</v>
+        <v>47.013210000000001</v>
       </c>
       <c r="E29" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="F29">
-        <v>54.158999999999999</v>
+        <v>47.786999999999999</v>
       </c>
       <c r="G29" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H29">
-        <v>5313</v>
+        <v>1412</v>
       </c>
       <c r="I29" t="s">
-        <v>291</v>
+        <v>122</v>
       </c>
       <c r="J29" t="s">
-        <v>290</v>
+        <v>123</v>
       </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M29" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="N29" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O29">
-        <v>19840</v>
+        <v>133952</v>
       </c>
       <c r="P29" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="R29">
-        <v>10.41</v>
+        <v>27.08</v>
       </c>
       <c r="S29">
-        <f>2.9091*R29</f>
-        <v>30.283731</v>
+        <f t="shared" si="0"/>
+        <v>78.778427999999991</v>
       </c>
       <c r="T29">
-        <f>1.92*R29</f>
-        <v>19.987199999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>51.993599999999994</v>
+      </c>
+      <c r="U29" s="5">
+        <v>58.431399999999996</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="2"/>
+        <v>88.231414000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1303</v>
       </c>
@@ -3173,15 +3381,22 @@
         <v>32.82</v>
       </c>
       <c r="S30">
-        <f>2.9091*R30</f>
+        <f t="shared" si="0"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T30">
-        <f>1.92*R30</f>
+        <f t="shared" si="1"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U30" s="5">
+        <v>63.75</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="2"/>
+        <v>96.262500000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1574</v>
       </c>
@@ -3231,15 +3446,22 @@
         <v>32.82</v>
       </c>
       <c r="S31">
-        <f>2.9091*R31</f>
+        <f t="shared" si="0"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T31">
-        <f>1.92*R31</f>
+        <f t="shared" si="1"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U31" s="5">
+        <v>64.409099999999995</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="2"/>
+        <v>97.257740999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1720</v>
       </c>
@@ -3289,15 +3511,22 @@
         <v>11.452999999999999</v>
       </c>
       <c r="S32">
-        <f>2.9091*R32</f>
+        <f t="shared" si="0"/>
         <v>33.317922299999999</v>
       </c>
       <c r="T32">
-        <f>1.92*R32</f>
+        <f t="shared" si="1"/>
         <v>21.989759999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U32" s="5">
+        <v>54.909500000000001</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="2"/>
+        <v>82.913345000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1721</v>
       </c>
@@ -3347,15 +3576,22 @@
         <v>32.82</v>
       </c>
       <c r="S33">
-        <f>2.9091*R33</f>
+        <f t="shared" si="0"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T33">
-        <f>1.92*R33</f>
+        <f t="shared" si="1"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U33" s="5">
+        <v>52.325000000000003</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="2"/>
+        <v>79.010750000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1746</v>
       </c>
@@ -3408,15 +3644,22 @@
         <v>32.82</v>
       </c>
       <c r="S34">
-        <f>2.9091*R34</f>
+        <f t="shared" ref="S34:S65" si="3">2.9091*R34</f>
         <v>95.476662000000005</v>
       </c>
       <c r="T34">
-        <f>1.92*R34</f>
+        <f t="shared" ref="T34:T65" si="4">1.92*R34</f>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U34" s="5">
+        <v>61.088900000000002</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="2"/>
+        <v>92.244239000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1781</v>
       </c>
@@ -3469,15 +3712,22 @@
         <v>32.82</v>
       </c>
       <c r="S35">
-        <f>2.9091*R35</f>
+        <f t="shared" si="3"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T35">
-        <f>1.92*R35</f>
+        <f t="shared" si="4"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U35" s="5">
+        <v>48.428600000000003</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="2"/>
+        <v>73.127186000000009</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1806</v>
       </c>
@@ -3530,15 +3780,22 @@
         <v>6.68</v>
       </c>
       <c r="S36">
-        <f>2.9091*R36</f>
+        <f t="shared" si="3"/>
         <v>19.432787999999999</v>
       </c>
       <c r="T36">
-        <f>1.92*R36</f>
+        <f t="shared" si="4"/>
         <v>12.8256</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U36" s="5">
+        <v>13.2798</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="2"/>
+        <v>20.052498</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1812</v>
       </c>
@@ -3591,15 +3848,22 @@
         <v>32.82</v>
       </c>
       <c r="S37">
-        <f>2.9091*R37</f>
+        <f t="shared" si="3"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T37">
-        <f>1.92*R37</f>
+        <f t="shared" si="4"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U37" s="5">
+        <v>52.625</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="2"/>
+        <v>79.463750000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1821</v>
       </c>
@@ -3652,15 +3916,22 @@
         <v>6.68</v>
       </c>
       <c r="S38">
-        <f>2.9091*R38</f>
+        <f t="shared" si="3"/>
         <v>19.432787999999999</v>
       </c>
       <c r="T38">
-        <f>1.92*R38</f>
+        <f t="shared" si="4"/>
         <v>12.8256</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U38" s="5">
+        <v>13.2432</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="2"/>
+        <v>19.997232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1842</v>
       </c>
@@ -3713,15 +3984,22 @@
         <v>32.82</v>
       </c>
       <c r="S39">
-        <f>2.9091*R39</f>
+        <f t="shared" si="3"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T39">
-        <f>1.92*R39</f>
+        <f t="shared" si="4"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U39" s="5">
+        <v>63</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="2"/>
+        <v>95.13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1863</v>
       </c>
@@ -3774,15 +4052,22 @@
         <v>32.82</v>
       </c>
       <c r="S40">
-        <f>2.9091*R40</f>
+        <f t="shared" si="3"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T40">
-        <f>1.92*R40</f>
+        <f t="shared" si="4"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U40" s="5">
+        <v>53.130400000000002</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="2"/>
+        <v>80.226904000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2063</v>
       </c>
@@ -3832,15 +4117,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S41">
-        <f>2.9091*R41</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T41">
-        <f>1.92*R41</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U41" s="5">
+        <v>51.428600000000003</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="2"/>
+        <v>77.65718600000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2071</v>
       </c>
@@ -3890,15 +4182,22 @@
         <v>11.452999999999999</v>
       </c>
       <c r="S42">
-        <f>2.9091*R42</f>
+        <f t="shared" si="3"/>
         <v>33.317922299999999</v>
       </c>
       <c r="T42">
-        <f>1.92*R42</f>
+        <f t="shared" si="4"/>
         <v>21.989759999999997</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U42" s="5">
+        <v>57.265799999999999</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="2"/>
+        <v>86.471357999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2128</v>
       </c>
@@ -3951,15 +4250,22 @@
         <v>29.68</v>
       </c>
       <c r="S43">
-        <f>2.9091*R43</f>
+        <f t="shared" si="3"/>
         <v>86.342088000000004</v>
       </c>
       <c r="T43">
-        <f>1.92*R43</f>
+        <f t="shared" si="4"/>
         <v>56.985599999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U43" s="5">
+        <v>55.05</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="2"/>
+        <v>83.125500000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2132</v>
       </c>
@@ -4009,15 +4315,22 @@
         <v>29.68</v>
       </c>
       <c r="S44">
-        <f>2.9091*R44</f>
+        <f t="shared" si="3"/>
         <v>86.342088000000004</v>
       </c>
       <c r="T44">
-        <f>1.92*R44</f>
+        <f t="shared" si="4"/>
         <v>56.985599999999998</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U44" s="5">
+        <v>51</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="2"/>
+        <v>77.010000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2165</v>
       </c>
@@ -4070,15 +4383,22 @@
         <v>99.479200000000006</v>
       </c>
       <c r="S45">
-        <f>2.9091*R45</f>
+        <f t="shared" si="3"/>
         <v>289.39494072000002</v>
       </c>
       <c r="T45">
-        <f>1.92*R45</f>
+        <f t="shared" si="4"/>
         <v>191.00006400000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U45">
+        <v>191</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="2"/>
+        <v>288.41000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2170</v>
       </c>
@@ -4131,15 +4451,22 @@
         <v>50</v>
       </c>
       <c r="S46">
-        <f>2.9091*R46</f>
+        <f t="shared" si="3"/>
         <v>145.45500000000001</v>
       </c>
       <c r="T46">
-        <f>1.92*R46</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U46" s="5">
+        <v>49.094000000000001</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="2"/>
+        <v>74.13194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2171</v>
       </c>
@@ -4195,15 +4522,22 @@
         <v>99.479200000000006</v>
       </c>
       <c r="S47">
-        <f>2.9091*R47</f>
+        <f t="shared" si="3"/>
         <v>289.39494072000002</v>
       </c>
       <c r="T47">
-        <f>1.92*R47</f>
+        <f t="shared" si="4"/>
         <v>191.00006400000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U47">
+        <v>191</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="2"/>
+        <v>288.41000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2178</v>
       </c>
@@ -4256,15 +4590,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S48">
-        <f>2.9091*R48</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T48">
-        <f>1.92*R48</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U48" s="5">
+        <v>52.896599999999999</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="2"/>
+        <v>79.873865999999992</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2183</v>
       </c>
@@ -4317,15 +4658,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S49">
-        <f>2.9091*R49</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T49">
-        <f>1.92*R49</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U49" s="5">
+        <v>54.84</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="2"/>
+        <v>82.808400000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2185</v>
       </c>
@@ -4378,15 +4726,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S50">
-        <f>2.9091*R50</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T50">
-        <f>1.92*R50</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U50" s="5">
+        <v>50.486499999999999</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="2"/>
+        <v>76.234615000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2209</v>
       </c>
@@ -4439,15 +4794,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S51">
-        <f>2.9091*R51</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T51">
-        <f>1.92*R51</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U51" s="5">
+        <v>54.971400000000003</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="2"/>
+        <v>83.006814000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2232</v>
       </c>
@@ -4500,15 +4862,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S52">
-        <f>2.9091*R52</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T52">
-        <f>1.92*R52</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U52" s="5">
+        <v>76.650000000000006</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="2"/>
+        <v>115.74150000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2242</v>
       </c>
@@ -4561,15 +4930,22 @@
         <v>33.33</v>
       </c>
       <c r="S53">
-        <f>2.9091*R53</f>
+        <f t="shared" si="3"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T53">
-        <f>1.92*R53</f>
+        <f t="shared" si="4"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U53" s="5">
+        <v>62.521700000000003</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="2"/>
+        <v>94.407767000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2266</v>
       </c>
@@ -4619,15 +4995,22 @@
         <v>27.08</v>
       </c>
       <c r="S54">
-        <f>2.9091*R54</f>
+        <f t="shared" si="3"/>
         <v>78.778427999999991</v>
       </c>
       <c r="T54">
-        <f>1.92*R54</f>
+        <f t="shared" si="4"/>
         <v>51.993599999999994</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U54" s="5">
+        <v>52</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="2"/>
+        <v>78.52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2289</v>
       </c>
@@ -4680,15 +5063,22 @@
         <v>32.82</v>
       </c>
       <c r="S55">
-        <f>2.9091*R55</f>
+        <f t="shared" si="3"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T55">
-        <f>1.92*R55</f>
+        <f t="shared" si="4"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U55" s="5">
+        <v>61.5</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="2"/>
+        <v>92.864999999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2294</v>
       </c>
@@ -4741,15 +5131,22 @@
         <v>11.452999999999999</v>
       </c>
       <c r="S56">
-        <f>2.9091*R56</f>
+        <f t="shared" si="3"/>
         <v>33.317922299999999</v>
       </c>
       <c r="T56">
-        <f>1.92*R56</f>
+        <f t="shared" si="4"/>
         <v>21.989759999999997</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U56" s="5">
+        <v>62.244399999999999</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="2"/>
+        <v>93.989043999999993</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2308</v>
       </c>
@@ -4802,15 +5199,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S57">
-        <f>2.9091*R57</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T57">
-        <f>1.92*R57</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U57" s="5">
+        <v>52.567599999999999</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="2"/>
+        <v>79.377076000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2321</v>
       </c>
@@ -4863,15 +5267,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S58">
-        <f>2.9091*R58</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T58">
-        <f>1.92*R58</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U58" s="5">
+        <v>55.214300000000001</v>
+      </c>
+      <c r="V58">
+        <f t="shared" si="2"/>
+        <v>83.373593</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2322</v>
       </c>
@@ -4924,15 +5335,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S59">
-        <f>2.9091*R59</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T59">
-        <f>1.92*R59</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U59" s="5">
+        <v>54.851900000000001</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="2"/>
+        <v>82.826369</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2323</v>
       </c>
@@ -4985,15 +5403,22 @@
         <v>10.41</v>
       </c>
       <c r="S60">
-        <f>2.9091*R60</f>
+        <f t="shared" si="3"/>
         <v>30.283731</v>
       </c>
       <c r="T60">
-        <f>1.92*R60</f>
+        <f t="shared" si="4"/>
         <v>19.987199999999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U60">
+        <v>20</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="2"/>
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2324</v>
       </c>
@@ -5046,15 +5471,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S61">
-        <f>2.9091*R61</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T61">
-        <f>1.92*R61</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U61">
+        <v>59</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="2"/>
+        <v>89.09</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>237</v>
       </c>
@@ -5107,15 +5539,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S62">
-        <f>2.9091*R62</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T62">
-        <f>1.92*R62</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U62" s="5">
+        <v>59</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="2"/>
+        <v>89.09</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>254</v>
       </c>
@@ -5168,15 +5607,22 @@
         <v>33.854199999999999</v>
       </c>
       <c r="S63">
-        <f>2.9091*R63</f>
+        <f t="shared" si="3"/>
         <v>98.48525321999999</v>
       </c>
       <c r="T63">
-        <f>1.92*R63</f>
+        <f t="shared" si="4"/>
         <v>65.000063999999995</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U63" s="5">
+        <v>67.136399999999995</v>
+      </c>
+      <c r="V63">
+        <f t="shared" si="2"/>
+        <v>101.375964</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>313</v>
       </c>
@@ -5226,15 +5672,22 @@
         <v>10.414999999999999</v>
       </c>
       <c r="S64">
-        <f>2.9091*R64</f>
+        <f t="shared" si="3"/>
         <v>30.298276499999997</v>
       </c>
       <c r="T64">
-        <f>1.92*R64</f>
+        <f t="shared" si="4"/>
         <v>19.996799999999997</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U64" s="5">
+        <v>25.7239</v>
+      </c>
+      <c r="V64">
+        <f t="shared" si="2"/>
+        <v>38.843088999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>382</v>
       </c>
@@ -5284,15 +5737,22 @@
         <v>23.43</v>
       </c>
       <c r="S65">
-        <f>2.9091*R65</f>
+        <f t="shared" si="3"/>
         <v>68.160212999999999</v>
       </c>
       <c r="T65">
-        <f>1.92*R65</f>
+        <f t="shared" si="4"/>
         <v>44.985599999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U65">
+        <v>45</v>
+      </c>
+      <c r="V65">
+        <f t="shared" si="2"/>
+        <v>67.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>385</v>
       </c>
@@ -5345,15 +5805,22 @@
         <v>23.43</v>
       </c>
       <c r="S66">
-        <f>2.9091*R66</f>
+        <f t="shared" ref="S66:S78" si="5">2.9091*R66</f>
         <v>68.160212999999999</v>
       </c>
       <c r="T66">
-        <f>1.92*R66</f>
+        <f t="shared" ref="T66:T78" si="6">1.92*R66</f>
         <v>44.985599999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U66">
+        <v>45</v>
+      </c>
+      <c r="V66">
+        <f t="shared" si="2"/>
+        <v>67.95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>408</v>
       </c>
@@ -5406,15 +5873,22 @@
         <v>33.33</v>
       </c>
       <c r="S67">
-        <f>2.9091*R67</f>
+        <f t="shared" si="5"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T67">
-        <f>1.92*R67</f>
+        <f t="shared" si="6"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U67" s="5">
+        <v>67.625</v>
+      </c>
+      <c r="V67">
+        <f t="shared" ref="V67:V78" si="7">U67*1.51</f>
+        <v>102.11375</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>405</v>
       </c>
@@ -5464,15 +5938,22 @@
         <v>33.33</v>
       </c>
       <c r="S68">
-        <f>2.9091*R68</f>
+        <f t="shared" si="5"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T68">
-        <f>1.92*R68</f>
+        <f t="shared" si="6"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U68" s="5">
+        <v>66.678600000000003</v>
+      </c>
+      <c r="V68">
+        <f t="shared" si="7"/>
+        <v>100.684686</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>922</v>
       </c>
@@ -5522,15 +6003,22 @@
         <v>10.41</v>
       </c>
       <c r="S69">
-        <f>2.9091*R69</f>
+        <f t="shared" si="5"/>
         <v>30.283731</v>
       </c>
       <c r="T69">
-        <f>1.92*R69</f>
+        <f t="shared" si="6"/>
         <v>19.987199999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U69">
+        <v>20</v>
+      </c>
+      <c r="V69">
+        <f t="shared" si="7"/>
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1098</v>
       </c>
@@ -5580,15 +6068,22 @@
         <v>20.83</v>
       </c>
       <c r="S70">
-        <f>2.9091*R70</f>
+        <f t="shared" si="5"/>
         <v>60.596552999999993</v>
       </c>
       <c r="T70">
-        <f>1.92*R70</f>
+        <f t="shared" si="6"/>
         <v>39.993599999999994</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U70" s="5">
+        <v>50.8</v>
+      </c>
+      <c r="V70">
+        <f t="shared" si="7"/>
+        <v>76.707999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>379</v>
       </c>
@@ -5638,15 +6133,22 @@
         <v>33.33</v>
       </c>
       <c r="S71">
-        <f>2.9091*R71</f>
+        <f t="shared" si="5"/>
         <v>96.960302999999996</v>
       </c>
       <c r="T71">
-        <f>1.92*R71</f>
+        <f t="shared" si="6"/>
         <v>63.993599999999994</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U71" s="5">
+        <v>57.661000000000001</v>
+      </c>
+      <c r="V71">
+        <f t="shared" si="7"/>
+        <v>87.068110000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1739</v>
       </c>
@@ -5696,15 +6198,22 @@
         <v>32.82</v>
       </c>
       <c r="S72">
-        <f>2.9091*R72</f>
+        <f t="shared" si="5"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T72">
-        <f>1.92*R72</f>
+        <f t="shared" si="6"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U72" s="5">
+        <v>53.477699999999999</v>
+      </c>
+      <c r="V72">
+        <f t="shared" si="7"/>
+        <v>80.751327000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1568</v>
       </c>
@@ -5754,15 +6263,22 @@
         <v>32.82</v>
       </c>
       <c r="S73">
-        <f>2.9091*R73</f>
+        <f t="shared" si="5"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T73">
-        <f>1.92*R73</f>
+        <f t="shared" si="6"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U73" s="5">
+        <v>54.022300000000001</v>
+      </c>
+      <c r="V73">
+        <f t="shared" si="7"/>
+        <v>81.573672999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1730</v>
       </c>
@@ -5815,15 +6331,22 @@
         <v>32.82</v>
       </c>
       <c r="S74">
-        <f>2.9091*R74</f>
+        <f t="shared" si="5"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T74">
-        <f>1.92*R74</f>
+        <f t="shared" si="6"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U74" s="5">
+        <v>54.545499999999997</v>
+      </c>
+      <c r="V74">
+        <f t="shared" si="7"/>
+        <v>82.363704999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1733</v>
       </c>
@@ -5876,15 +6399,22 @@
         <v>32.82</v>
       </c>
       <c r="S75">
-        <f>2.9091*R75</f>
+        <f t="shared" si="5"/>
         <v>95.476662000000005</v>
       </c>
       <c r="T75">
-        <f>1.92*R75</f>
+        <f t="shared" si="6"/>
         <v>63.014399999999995</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U75" s="5">
+        <v>55.192300000000003</v>
+      </c>
+      <c r="V75">
+        <f t="shared" si="7"/>
+        <v>83.340373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1593</v>
       </c>
@@ -5937,15 +6467,22 @@
         <v>41.6</v>
       </c>
       <c r="S76">
-        <f>2.9091*R76</f>
+        <f t="shared" si="5"/>
         <v>121.01856000000001</v>
       </c>
       <c r="T76">
-        <f>1.92*R76</f>
+        <f t="shared" si="6"/>
         <v>79.872</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U76" s="5">
+        <v>65.027000000000001</v>
+      </c>
+      <c r="V76">
+        <f t="shared" si="7"/>
+        <v>98.190770000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1599</v>
       </c>
@@ -5998,15 +6535,22 @@
         <v>41.6</v>
       </c>
       <c r="S77">
-        <f>2.9091*R77</f>
+        <f t="shared" si="5"/>
         <v>121.01856000000001</v>
       </c>
       <c r="T77">
-        <f>1.92*R77</f>
+        <f t="shared" si="6"/>
         <v>79.872</v>
       </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U77" s="5">
+        <v>62.65</v>
+      </c>
+      <c r="V77">
+        <f t="shared" si="7"/>
+        <v>94.601500000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1596</v>
       </c>
@@ -6059,12 +6603,19 @@
         <v>41.6</v>
       </c>
       <c r="S78">
-        <f>2.9091*R78</f>
+        <f t="shared" si="5"/>
         <v>121.01856000000001</v>
       </c>
       <c r="T78">
-        <f>1.92*R78</f>
+        <f t="shared" si="6"/>
         <v>79.872</v>
+      </c>
+      <c r="U78" s="5">
+        <v>49.094000000000001</v>
+      </c>
+      <c r="V78">
+        <f t="shared" si="7"/>
+        <v>74.13194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>